<commit_message>
Add - ejecución de red-unet
Los errores de validación aumentaron, pero siguen siendo cercanos a 0. Falta obtener el NMSE de la VSC original y predicha para observar la calidad de la red.
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\waveletycnn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\MemoriaCodigoFuentev3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65D5921-D05D-4916-9D38-5E6E2EB236A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990121DF-B134-4223-B2E9-C648A96B3D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="79">
   <si>
     <t>MODELO U-NET: FULL SIGNALS</t>
   </si>
@@ -288,6 +288,12 @@
   </si>
   <si>
     <t>unet_model_7.keras</t>
+  </si>
+  <si>
+    <t>unet_model_vscd_1_HEMU_v1.keras</t>
+  </si>
+  <si>
+    <t>unet_model_vscd_1_HEMU_v2.keras</t>
   </si>
 </sst>
 </file>
@@ -363,7 +369,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -466,6 +472,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -527,7 +539,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -772,6 +784,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3012,11 +3048,11 @@
   <sheetPr>
     <tabColor theme="3" tint="0.499984740745262"/>
   </sheetPr>
-  <dimension ref="B3:S19"/>
+  <dimension ref="B3:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3660,48 +3696,231 @@
       <c r="S17" s="77"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="73"/>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="71"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="71"/>
-      <c r="K18" s="71"/>
+      <c r="B18" s="86"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="87"/>
+      <c r="H18" s="87"/>
+      <c r="I18" s="87"/>
+      <c r="J18" s="87"/>
+      <c r="K18" s="87"/>
       <c r="L18" s="85"/>
-      <c r="M18" s="72"/>
-      <c r="N18" s="72"/>
-      <c r="O18" s="72"/>
-      <c r="P18" s="72"/>
+      <c r="M18" s="88"/>
+      <c r="N18" s="88"/>
+      <c r="O18" s="88"/>
+      <c r="P18" s="88"/>
       <c r="Q18" s="85"/>
-      <c r="R18" s="71"/>
+      <c r="R18" s="89"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="73"/>
-      <c r="C19" s="70"/>
-      <c r="D19" s="70"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="71"/>
-      <c r="I19" s="71"/>
-      <c r="J19" s="71"/>
-      <c r="K19" s="71"/>
+      <c r="B19" s="90" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="91">
+        <v>50</v>
+      </c>
+      <c r="D19" s="91" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="91"/>
+      <c r="F19" s="92">
+        <v>1E-3</v>
+      </c>
+      <c r="G19" s="92">
+        <v>300</v>
+      </c>
+      <c r="H19" s="92">
+        <v>8</v>
+      </c>
+      <c r="I19" s="92"/>
+      <c r="J19" s="92"/>
+      <c r="K19" s="92" t="s">
+        <v>6</v>
+      </c>
       <c r="L19" s="85"/>
-      <c r="M19" s="72"/>
-      <c r="N19" s="72"/>
-      <c r="O19" s="72"/>
-      <c r="P19" s="72"/>
+      <c r="M19" s="93">
+        <v>1.8E-3</v>
+      </c>
+      <c r="N19" s="93">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="O19" s="93">
+        <v>0.12709999999999999</v>
+      </c>
+      <c r="P19" s="93">
+        <v>0.3236</v>
+      </c>
       <c r="Q19" s="85"/>
-      <c r="R19" s="71"/>
+      <c r="R19" s="92">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B20" s="90" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="91">
+        <v>50</v>
+      </c>
+      <c r="D20" s="91" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="91"/>
+      <c r="F20" s="71">
+        <v>1E-4</v>
+      </c>
+      <c r="G20" s="71">
+        <v>200</v>
+      </c>
+      <c r="H20" s="71">
+        <v>8</v>
+      </c>
+      <c r="I20" s="71"/>
+      <c r="J20" s="71"/>
+      <c r="K20" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="L20" s="84"/>
+      <c r="M20" s="72">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="N20" s="72">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="O20" s="72">
+        <v>0.1351</v>
+      </c>
+      <c r="P20" s="72">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="Q20" s="84"/>
+      <c r="R20" s="71">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B21" s="90"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="91"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="71"/>
+      <c r="K21" s="71"/>
+      <c r="L21" s="85"/>
+      <c r="M21" s="72"/>
+      <c r="N21" s="72"/>
+      <c r="O21" s="72"/>
+      <c r="P21" s="72"/>
+      <c r="Q21" s="85"/>
+      <c r="R21" s="71"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B22" s="90"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="91"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="71"/>
+      <c r="J22" s="71"/>
+      <c r="K22" s="71"/>
+      <c r="L22" s="85"/>
+      <c r="M22" s="72"/>
+      <c r="N22" s="72"/>
+      <c r="O22" s="72"/>
+      <c r="P22" s="72"/>
+      <c r="Q22" s="85"/>
+      <c r="R22" s="71"/>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="90"/>
+      <c r="C23" s="91"/>
+      <c r="D23" s="91"/>
+      <c r="E23" s="91"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="71"/>
+      <c r="K23" s="71"/>
+      <c r="L23" s="85"/>
+      <c r="M23" s="72"/>
+      <c r="N23" s="72"/>
+      <c r="O23" s="72"/>
+      <c r="P23" s="72"/>
+      <c r="Q23" s="85"/>
+      <c r="R23" s="71"/>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="90"/>
+      <c r="C24" s="91"/>
+      <c r="D24" s="91"/>
+      <c r="E24" s="91"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="71"/>
+      <c r="L24" s="85"/>
+      <c r="M24" s="72"/>
+      <c r="N24" s="72"/>
+      <c r="O24" s="72"/>
+      <c r="P24" s="72"/>
+      <c r="Q24" s="85"/>
+      <c r="R24" s="71"/>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="90"/>
+      <c r="C25" s="91"/>
+      <c r="D25" s="91"/>
+      <c r="E25" s="91"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="71"/>
+      <c r="K25" s="71"/>
+      <c r="L25" s="85"/>
+      <c r="M25" s="72"/>
+      <c r="N25" s="72"/>
+      <c r="O25" s="72"/>
+      <c r="P25" s="72"/>
+      <c r="Q25" s="85"/>
+      <c r="R25" s="71"/>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B26" s="90"/>
+      <c r="C26" s="91"/>
+      <c r="D26" s="91"/>
+      <c r="E26" s="91"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="71"/>
+      <c r="L26" s="85"/>
+      <c r="M26" s="72"/>
+      <c r="N26" s="72"/>
+      <c r="O26" s="72"/>
+      <c r="P26" s="72"/>
+      <c r="Q26" s="85"/>
+      <c r="R26" s="71"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="L5:L19"/>
     <mergeCell ref="Q5:Q19"/>
+    <mergeCell ref="L20:L26"/>
+    <mergeCell ref="Q20:Q26"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add - probando hiperparametros y obtención de modelos
- falta el escalón para probar la calidad de la red
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\MemoriaCodigoFuentev3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACE9043-65A8-41A6-A8B3-1250AFF87E82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74BCAE3-C49C-4E8C-823D-648550E3272D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
+    <workbookView xWindow="1005" yWindow="10740" windowWidth="21600" windowHeight="7695" activeTab="2" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
   <sheets>
     <sheet name="full_signals - without decay" sheetId="1" r:id="rId1"/>
     <sheet name="full_signals - with decay" sheetId="2" r:id="rId2"/>
+    <sheet name="modelos por sujeto sano" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="83">
   <si>
     <t>MODELO U-NET: FULL SIGNALS</t>
   </si>
@@ -295,6 +296,18 @@
   <si>
     <t>unet_model_vscd_1_HEMU_v2.keras</t>
   </si>
+  <si>
+    <t>unet_model_vscd.keras</t>
+  </si>
+  <si>
+    <t>unet_model_vscdv2.keras</t>
+  </si>
+  <si>
+    <t>SUJETO SANO</t>
+  </si>
+  <si>
+    <t>1_HEMU</t>
+  </si>
 </sst>
 </file>
 
@@ -304,7 +317,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,8 +381,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -478,6 +498,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -539,7 +565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -786,6 +812,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -808,6 +840,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1177,24 +1215,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
     </row>
     <row r="4" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -1983,10 +2021,10 @@
       <c r="P23" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q23" s="89" t="s">
+      <c r="Q23" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="R23" s="90"/>
+      <c r="R23" s="92"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
@@ -2026,8 +2064,8 @@
       <c r="P24" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q24" s="91"/>
-      <c r="R24" s="90"/>
+      <c r="Q24" s="93"/>
+      <c r="R24" s="92"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
@@ -2067,8 +2105,8 @@
       <c r="P25" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q25" s="91"/>
-      <c r="R25" s="90"/>
+      <c r="Q25" s="93"/>
+      <c r="R25" s="92"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="18" t="s">
@@ -2108,8 +2146,8 @@
       <c r="P26" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q26" s="91"/>
-      <c r="R26" s="90"/>
+      <c r="Q26" s="93"/>
+      <c r="R26" s="92"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="29" t="s">
@@ -2149,8 +2187,8 @@
       <c r="P27" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q27" s="91"/>
-      <c r="R27" s="90"/>
+      <c r="Q27" s="93"/>
+      <c r="R27" s="92"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
@@ -2190,8 +2228,8 @@
       <c r="P28" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q28" s="91"/>
-      <c r="R28" s="90"/>
+      <c r="Q28" s="93"/>
+      <c r="R28" s="92"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
@@ -2231,8 +2269,8 @@
       <c r="P29" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="91"/>
-      <c r="R29" s="90"/>
+      <c r="Q29" s="93"/>
+      <c r="R29" s="92"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="18" t="s">
@@ -2272,8 +2310,8 @@
       <c r="P30" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q30" s="91"/>
-      <c r="R30" s="90"/>
+      <c r="Q30" s="93"/>
+      <c r="R30" s="92"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
@@ -2313,8 +2351,8 @@
       <c r="P31" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q31" s="91"/>
-      <c r="R31" s="90"/>
+      <c r="Q31" s="93"/>
+      <c r="R31" s="92"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="29" t="s">
@@ -2354,8 +2392,8 @@
       <c r="P32" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q32" s="91"/>
-      <c r="R32" s="90"/>
+      <c r="Q32" s="93"/>
+      <c r="R32" s="92"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
@@ -2395,8 +2433,8 @@
       <c r="P33" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q33" s="91"/>
-      <c r="R33" s="90"/>
+      <c r="Q33" s="93"/>
+      <c r="R33" s="92"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
@@ -2436,8 +2474,8 @@
       <c r="P34" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q34" s="91"/>
-      <c r="R34" s="90"/>
+      <c r="Q34" s="93"/>
+      <c r="R34" s="92"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="18" t="s">
@@ -2477,8 +2515,8 @@
       <c r="P35" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q35" s="91"/>
-      <c r="R35" s="90"/>
+      <c r="Q35" s="93"/>
+      <c r="R35" s="92"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="18" t="s">
@@ -2518,8 +2556,8 @@
       <c r="P36" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q36" s="91"/>
-      <c r="R36" s="90"/>
+      <c r="Q36" s="93"/>
+      <c r="R36" s="92"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="29" t="s">
@@ -2559,21 +2597,21 @@
       <c r="P37" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q37" s="91"/>
-      <c r="R37" s="90"/>
+      <c r="Q37" s="93"/>
+      <c r="R37" s="92"/>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B39" s="88" t="s">
+      <c r="B39" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="88"/>
-      <c r="D39" s="88"/>
-      <c r="E39" s="88"/>
-      <c r="F39" s="88"/>
-      <c r="G39" s="88"/>
-      <c r="H39" s="88"/>
-      <c r="I39" s="88"/>
-      <c r="J39" s="88"/>
+      <c r="C39" s="90"/>
+      <c r="D39" s="90"/>
+      <c r="E39" s="90"/>
+      <c r="F39" s="90"/>
+      <c r="G39" s="90"/>
+      <c r="H39" s="90"/>
+      <c r="I39" s="90"/>
+      <c r="J39" s="90"/>
     </row>
     <row r="40" spans="2:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="49" t="s">
@@ -3050,9 +3088,9 @@
   </sheetPr>
   <dimension ref="B3:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5:R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3071,10 +3109,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="86"/>
+      <c r="C3" s="88"/>
     </row>
     <row r="5" spans="2:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="69" t="s">
@@ -3107,7 +3145,7 @@
       <c r="K5" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="92"/>
+      <c r="L5" s="94"/>
       <c r="M5" s="69" t="s">
         <v>7</v>
       </c>
@@ -3120,7 +3158,7 @@
       <c r="P5" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" s="92"/>
+      <c r="Q5" s="94"/>
       <c r="R5" s="69" t="s">
         <v>56</v>
       </c>
@@ -3153,7 +3191,7 @@
       <c r="K6" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="93"/>
+      <c r="L6" s="95"/>
       <c r="M6" s="72">
         <v>7.1400000000000005E-2</v>
       </c>
@@ -3166,7 +3204,7 @@
       <c r="P6" s="72">
         <v>0.16400000000000001</v>
       </c>
-      <c r="Q6" s="93"/>
+      <c r="Q6" s="95"/>
       <c r="R6" s="71">
         <v>116</v>
       </c>
@@ -3201,7 +3239,7 @@
       <c r="K7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="93"/>
+      <c r="L7" s="95"/>
       <c r="M7" s="75">
         <v>4.5789</v>
       </c>
@@ -3214,7 +3252,7 @@
       <c r="P7" s="75">
         <v>0.2122</v>
       </c>
-      <c r="Q7" s="93"/>
+      <c r="Q7" s="95"/>
       <c r="R7" s="6">
         <v>120</v>
       </c>
@@ -3249,7 +3287,7 @@
       <c r="K8" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="93"/>
+      <c r="L8" s="95"/>
       <c r="M8" s="72">
         <v>6.4744999999999999</v>
       </c>
@@ -3262,7 +3300,7 @@
       <c r="P8" s="72">
         <v>0.30930000000000002</v>
       </c>
-      <c r="Q8" s="93"/>
+      <c r="Q8" s="95"/>
       <c r="R8" s="71">
         <v>116</v>
       </c>
@@ -3297,7 +3335,7 @@
       <c r="K9" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L9" s="93"/>
+      <c r="L9" s="95"/>
       <c r="M9" s="72">
         <v>8.9992000000000001</v>
       </c>
@@ -3310,7 +3348,7 @@
       <c r="P9" s="72">
         <v>0.46489999999999998</v>
       </c>
-      <c r="Q9" s="93"/>
+      <c r="Q9" s="95"/>
       <c r="R9" s="71">
         <v>131</v>
       </c>
@@ -3345,7 +3383,7 @@
       <c r="K10" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="93"/>
+      <c r="L10" s="95"/>
       <c r="M10" s="72">
         <v>4.3776000000000002</v>
       </c>
@@ -3358,7 +3396,7 @@
       <c r="P10" s="72">
         <v>0.25719999999999998</v>
       </c>
-      <c r="Q10" s="93"/>
+      <c r="Q10" s="95"/>
       <c r="R10" s="71">
         <v>179</v>
       </c>
@@ -3393,7 +3431,7 @@
       <c r="K11" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="93"/>
+      <c r="L11" s="95"/>
       <c r="M11" s="72">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -3406,7 +3444,7 @@
       <c r="P11" s="72">
         <v>0.26069999999999999</v>
       </c>
-      <c r="Q11" s="93"/>
+      <c r="Q11" s="95"/>
       <c r="R11" s="71">
         <v>182</v>
       </c>
@@ -3441,7 +3479,7 @@
       <c r="K12" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="93"/>
+      <c r="L12" s="95"/>
       <c r="M12" s="72">
         <v>3.5999999999999999E-3</v>
       </c>
@@ -3454,7 +3492,7 @@
       <c r="P12" s="72">
         <v>0.39300000000000002</v>
       </c>
-      <c r="Q12" s="93"/>
+      <c r="Q12" s="95"/>
       <c r="R12" s="71">
         <v>89</v>
       </c>
@@ -3491,7 +3529,7 @@
       <c r="K13" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L13" s="93"/>
+      <c r="L13" s="95"/>
       <c r="M13" s="72">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -3504,7 +3542,7 @@
       <c r="P13" s="72">
         <v>0.41399999999999998</v>
       </c>
-      <c r="Q13" s="93"/>
+      <c r="Q13" s="95"/>
       <c r="R13" s="71">
         <v>44</v>
       </c>
@@ -3539,7 +3577,7 @@
       <c r="K14" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L14" s="93"/>
+      <c r="L14" s="95"/>
       <c r="M14" s="72">
         <v>1.1584000000000001</v>
       </c>
@@ -3552,7 +3590,7 @@
       <c r="P14" s="72">
         <v>0.1976</v>
       </c>
-      <c r="Q14" s="93"/>
+      <c r="Q14" s="95"/>
       <c r="R14" s="71">
         <v>305</v>
       </c>
@@ -3586,7 +3624,7 @@
       <c r="K15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L15" s="93"/>
+      <c r="L15" s="95"/>
       <c r="M15" s="75">
         <v>0.17349999999999999</v>
       </c>
@@ -3599,7 +3637,7 @@
       <c r="P15" s="75">
         <v>0.19939999999999999</v>
       </c>
-      <c r="Q15" s="93"/>
+      <c r="Q15" s="95"/>
       <c r="R15" s="6">
         <v>118</v>
       </c>
@@ -3633,7 +3671,7 @@
       <c r="K16" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L16" s="93"/>
+      <c r="L16" s="95"/>
       <c r="M16" s="72">
         <v>8.2579999999999991</v>
       </c>
@@ -3646,7 +3684,7 @@
       <c r="P16" s="72">
         <v>0.47870000000000001</v>
       </c>
-      <c r="Q16" s="93"/>
+      <c r="Q16" s="95"/>
       <c r="R16" s="71">
         <v>127</v>
       </c>
@@ -3676,7 +3714,7 @@
       <c r="K17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L17" s="93"/>
+      <c r="L17" s="95"/>
       <c r="M17" s="75">
         <v>3.5000000000000001E-3</v>
       </c>
@@ -3689,7 +3727,7 @@
       <c r="P17" s="75">
         <v>0.1825</v>
       </c>
-      <c r="Q17" s="93"/>
+      <c r="Q17" s="95"/>
       <c r="R17" s="6">
         <v>132</v>
       </c>
@@ -3706,12 +3744,12 @@
       <c r="I18" s="79"/>
       <c r="J18" s="79"/>
       <c r="K18" s="79"/>
-      <c r="L18" s="93"/>
+      <c r="L18" s="95"/>
       <c r="M18" s="80"/>
       <c r="N18" s="80"/>
       <c r="O18" s="80"/>
       <c r="P18" s="80"/>
-      <c r="Q18" s="93"/>
+      <c r="Q18" s="95"/>
       <c r="R18" s="81"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
@@ -3739,7 +3777,7 @@
       <c r="K19" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="L19" s="93"/>
+      <c r="L19" s="95"/>
       <c r="M19" s="85">
         <v>1.8E-3</v>
       </c>
@@ -3752,7 +3790,7 @@
       <c r="P19" s="85">
         <v>0.3236</v>
       </c>
-      <c r="Q19" s="93"/>
+      <c r="Q19" s="95"/>
       <c r="R19" s="84">
         <v>117</v>
       </c>
@@ -3782,7 +3820,7 @@
       <c r="K20" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L20" s="92"/>
+      <c r="L20" s="94"/>
       <c r="M20" s="72">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -3795,7 +3833,7 @@
       <c r="P20" s="72">
         <v>0.34599999999999997</v>
       </c>
-      <c r="Q20" s="92"/>
+      <c r="Q20" s="94"/>
       <c r="R20" s="71">
         <v>77</v>
       </c>
@@ -3811,12 +3849,12 @@
       <c r="I21" s="71"/>
       <c r="J21" s="71"/>
       <c r="K21" s="71"/>
-      <c r="L21" s="93"/>
+      <c r="L21" s="95"/>
       <c r="M21" s="72"/>
       <c r="N21" s="72"/>
       <c r="O21" s="72"/>
       <c r="P21" s="72"/>
-      <c r="Q21" s="93"/>
+      <c r="Q21" s="95"/>
       <c r="R21" s="71"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
@@ -3830,12 +3868,12 @@
       <c r="I22" s="71"/>
       <c r="J22" s="71"/>
       <c r="K22" s="71"/>
-      <c r="L22" s="93"/>
+      <c r="L22" s="95"/>
       <c r="M22" s="72"/>
       <c r="N22" s="72"/>
       <c r="O22" s="72"/>
       <c r="P22" s="72"/>
-      <c r="Q22" s="93"/>
+      <c r="Q22" s="95"/>
       <c r="R22" s="71"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
@@ -3849,12 +3887,12 @@
       <c r="I23" s="71"/>
       <c r="J23" s="71"/>
       <c r="K23" s="71"/>
-      <c r="L23" s="93"/>
+      <c r="L23" s="95"/>
       <c r="M23" s="72"/>
       <c r="N23" s="72"/>
       <c r="O23" s="72"/>
       <c r="P23" s="72"/>
-      <c r="Q23" s="93"/>
+      <c r="Q23" s="95"/>
       <c r="R23" s="71"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
@@ -3868,12 +3906,12 @@
       <c r="I24" s="71"/>
       <c r="J24" s="71"/>
       <c r="K24" s="71"/>
-      <c r="L24" s="93"/>
+      <c r="L24" s="95"/>
       <c r="M24" s="72"/>
       <c r="N24" s="72"/>
       <c r="O24" s="72"/>
       <c r="P24" s="72"/>
-      <c r="Q24" s="93"/>
+      <c r="Q24" s="95"/>
       <c r="R24" s="71"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
@@ -3887,12 +3925,12 @@
       <c r="I25" s="71"/>
       <c r="J25" s="71"/>
       <c r="K25" s="71"/>
-      <c r="L25" s="93"/>
+      <c r="L25" s="95"/>
       <c r="M25" s="72"/>
       <c r="N25" s="72"/>
       <c r="O25" s="72"/>
       <c r="P25" s="72"/>
-      <c r="Q25" s="93"/>
+      <c r="Q25" s="95"/>
       <c r="R25" s="71"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
@@ -3906,12 +3944,12 @@
       <c r="I26" s="71"/>
       <c r="J26" s="71"/>
       <c r="K26" s="71"/>
-      <c r="L26" s="93"/>
+      <c r="L26" s="95"/>
       <c r="M26" s="72"/>
       <c r="N26" s="72"/>
       <c r="O26" s="72"/>
       <c r="P26" s="72"/>
-      <c r="Q26" s="93"/>
+      <c r="Q26" s="95"/>
       <c r="R26" s="71"/>
     </row>
   </sheetData>
@@ -3925,4 +3963,331 @@
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83DACCE0-796E-4D65-A099-858508568136}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="B3:S13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="59.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="B3" s="97" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="96" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="96" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="96" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="96" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="96" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="96" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" s="96" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="96" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="86"/>
+      <c r="N3" s="96" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" s="96" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" s="96" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="96" t="s">
+        <v>10</v>
+      </c>
+      <c r="R3" s="86"/>
+      <c r="S3" s="96" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B4" s="71" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="71" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="71">
+        <v>50</v>
+      </c>
+      <c r="E4" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71">
+        <v>1E-3</v>
+      </c>
+      <c r="H4" s="71">
+        <v>300</v>
+      </c>
+      <c r="I4" s="71">
+        <v>8</v>
+      </c>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="87"/>
+      <c r="N4" s="72">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="O4" s="72">
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="P4" s="72">
+        <v>0.13270000000000001</v>
+      </c>
+      <c r="Q4" s="72">
+        <v>0.33829999999999999</v>
+      </c>
+      <c r="R4" s="87"/>
+      <c r="S4" s="71">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="71" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="71" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="71">
+        <v>50</v>
+      </c>
+      <c r="E5" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71">
+        <v>1E-4</v>
+      </c>
+      <c r="H5" s="71">
+        <v>300</v>
+      </c>
+      <c r="I5" s="71">
+        <v>8</v>
+      </c>
+      <c r="J5" s="71"/>
+      <c r="K5" s="71"/>
+      <c r="L5" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="87"/>
+      <c r="N5" s="72">
+        <v>1.9E-3</v>
+      </c>
+      <c r="O5" s="72">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="P5" s="72">
+        <v>0.12</v>
+      </c>
+      <c r="Q5" s="72">
+        <v>0.31059999999999999</v>
+      </c>
+      <c r="R5" s="87"/>
+      <c r="S5" s="71">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="71"/>
+      <c r="L6" s="71"/>
+      <c r="M6" s="87"/>
+      <c r="N6" s="72"/>
+      <c r="O6" s="72"/>
+      <c r="P6" s="72"/>
+      <c r="Q6" s="72"/>
+      <c r="R6" s="87"/>
+      <c r="S6" s="71"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="71"/>
+      <c r="K7" s="71"/>
+      <c r="L7" s="71"/>
+      <c r="M7" s="87"/>
+      <c r="N7" s="72"/>
+      <c r="O7" s="72"/>
+      <c r="P7" s="72"/>
+      <c r="Q7" s="72"/>
+      <c r="R7" s="87"/>
+      <c r="S7" s="71"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="71"/>
+      <c r="M8" s="87"/>
+      <c r="N8" s="72"/>
+      <c r="O8" s="72"/>
+      <c r="P8" s="72"/>
+      <c r="Q8" s="72"/>
+      <c r="R8" s="87"/>
+      <c r="S8" s="71"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="71"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="71"/>
+      <c r="L9" s="71"/>
+      <c r="M9" s="87"/>
+      <c r="N9" s="72"/>
+      <c r="O9" s="72"/>
+      <c r="P9" s="72"/>
+      <c r="Q9" s="72"/>
+      <c r="R9" s="87"/>
+      <c r="S9" s="71"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="71"/>
+      <c r="L10" s="71"/>
+      <c r="M10" s="87"/>
+      <c r="N10" s="72"/>
+      <c r="O10" s="72"/>
+      <c r="P10" s="72"/>
+      <c r="Q10" s="72"/>
+      <c r="R10" s="87"/>
+      <c r="S10" s="71"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B11" s="71"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="71"/>
+      <c r="M11" s="87"/>
+      <c r="N11" s="72"/>
+      <c r="O11" s="72"/>
+      <c r="P11" s="72"/>
+      <c r="Q11" s="72"/>
+      <c r="R11" s="87"/>
+      <c r="S11" s="71"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="71"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="87"/>
+      <c r="N12" s="72"/>
+      <c r="O12" s="72"/>
+      <c r="P12" s="72"/>
+      <c r="Q12" s="72"/>
+      <c r="R12" s="87"/>
+      <c r="S12" s="71"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="71"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="71"/>
+      <c r="J13" s="71"/>
+      <c r="K13" s="71"/>
+      <c r="L13" s="71"/>
+      <c r="M13" s="87"/>
+      <c r="N13" s="72"/>
+      <c r="O13" s="72"/>
+      <c r="P13" s="72"/>
+      <c r="Q13" s="72"/>
+      <c r="R13" s="87"/>
+      <c r="S13" s="71"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add - guardado de distintas versiones de modelos y métricas asociadas
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\MemoriaCodigoFuentev3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74BCAE3-C49C-4E8C-823D-648550E3272D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A70DCF-119E-4272-9C00-68D9D08C6B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1005" yWindow="10740" windowWidth="21600" windowHeight="7695" activeTab="2" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
+    <workbookView xWindow="3135" yWindow="7710" windowWidth="21600" windowHeight="7695" activeTab="2" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
   <sheets>
     <sheet name="full_signals - without decay" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="87">
   <si>
     <t>MODELO U-NET: FULL SIGNALS</t>
   </si>
@@ -307,6 +307,18 @@
   </si>
   <si>
     <t>1_HEMU</t>
+  </si>
+  <si>
+    <t>unet_model_vscdv3.keras</t>
+  </si>
+  <si>
+    <t>unet_model_vscdv4.keras</t>
+  </si>
+  <si>
+    <t>unet_model_vscdv5.keras</t>
+  </si>
+  <si>
+    <t>unet_model_vscdv6.keras</t>
   </si>
 </sst>
 </file>
@@ -818,6 +830,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -840,12 +858,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1193,7 +1205,7 @@
   </sheetPr>
   <dimension ref="B2:R54"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A28" sqref="A28:XFD32"/>
     </sheetView>
   </sheetViews>
@@ -1215,24 +1227,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
     </row>
     <row r="4" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -2021,10 +2033,10 @@
       <c r="P23" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q23" s="91" t="s">
+      <c r="Q23" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="R23" s="92"/>
+      <c r="R23" s="94"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
@@ -2064,8 +2076,8 @@
       <c r="P24" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q24" s="93"/>
-      <c r="R24" s="92"/>
+      <c r="Q24" s="95"/>
+      <c r="R24" s="94"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
@@ -2105,8 +2117,8 @@
       <c r="P25" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q25" s="93"/>
-      <c r="R25" s="92"/>
+      <c r="Q25" s="95"/>
+      <c r="R25" s="94"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="18" t="s">
@@ -2146,8 +2158,8 @@
       <c r="P26" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q26" s="93"/>
-      <c r="R26" s="92"/>
+      <c r="Q26" s="95"/>
+      <c r="R26" s="94"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="29" t="s">
@@ -2187,8 +2199,8 @@
       <c r="P27" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q27" s="93"/>
-      <c r="R27" s="92"/>
+      <c r="Q27" s="95"/>
+      <c r="R27" s="94"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
@@ -2228,8 +2240,8 @@
       <c r="P28" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q28" s="93"/>
-      <c r="R28" s="92"/>
+      <c r="Q28" s="95"/>
+      <c r="R28" s="94"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
@@ -2269,8 +2281,8 @@
       <c r="P29" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="93"/>
-      <c r="R29" s="92"/>
+      <c r="Q29" s="95"/>
+      <c r="R29" s="94"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="18" t="s">
@@ -2310,8 +2322,8 @@
       <c r="P30" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q30" s="93"/>
-      <c r="R30" s="92"/>
+      <c r="Q30" s="95"/>
+      <c r="R30" s="94"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
@@ -2351,8 +2363,8 @@
       <c r="P31" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q31" s="93"/>
-      <c r="R31" s="92"/>
+      <c r="Q31" s="95"/>
+      <c r="R31" s="94"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="29" t="s">
@@ -2392,8 +2404,8 @@
       <c r="P32" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q32" s="93"/>
-      <c r="R32" s="92"/>
+      <c r="Q32" s="95"/>
+      <c r="R32" s="94"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
@@ -2433,8 +2445,8 @@
       <c r="P33" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q33" s="93"/>
-      <c r="R33" s="92"/>
+      <c r="Q33" s="95"/>
+      <c r="R33" s="94"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
@@ -2474,8 +2486,8 @@
       <c r="P34" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q34" s="93"/>
-      <c r="R34" s="92"/>
+      <c r="Q34" s="95"/>
+      <c r="R34" s="94"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="18" t="s">
@@ -2515,8 +2527,8 @@
       <c r="P35" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q35" s="93"/>
-      <c r="R35" s="92"/>
+      <c r="Q35" s="95"/>
+      <c r="R35" s="94"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="18" t="s">
@@ -2556,8 +2568,8 @@
       <c r="P36" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q36" s="93"/>
-      <c r="R36" s="92"/>
+      <c r="Q36" s="95"/>
+      <c r="R36" s="94"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="29" t="s">
@@ -2597,21 +2609,21 @@
       <c r="P37" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q37" s="93"/>
-      <c r="R37" s="92"/>
+      <c r="Q37" s="95"/>
+      <c r="R37" s="94"/>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B39" s="90" t="s">
+      <c r="B39" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="90"/>
-      <c r="D39" s="90"/>
-      <c r="E39" s="90"/>
-      <c r="F39" s="90"/>
-      <c r="G39" s="90"/>
-      <c r="H39" s="90"/>
-      <c r="I39" s="90"/>
-      <c r="J39" s="90"/>
+      <c r="C39" s="92"/>
+      <c r="D39" s="92"/>
+      <c r="E39" s="92"/>
+      <c r="F39" s="92"/>
+      <c r="G39" s="92"/>
+      <c r="H39" s="92"/>
+      <c r="I39" s="92"/>
+      <c r="J39" s="92"/>
     </row>
     <row r="40" spans="2:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="49" t="s">
@@ -3089,8 +3101,8 @@
   <dimension ref="B3:S26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5:R19"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3109,10 +3121,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="88"/>
+      <c r="C3" s="90"/>
     </row>
     <row r="5" spans="2:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="69" t="s">
@@ -3145,7 +3157,7 @@
       <c r="K5" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="94"/>
+      <c r="L5" s="96"/>
       <c r="M5" s="69" t="s">
         <v>7</v>
       </c>
@@ -3158,7 +3170,7 @@
       <c r="P5" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" s="94"/>
+      <c r="Q5" s="96"/>
       <c r="R5" s="69" t="s">
         <v>56</v>
       </c>
@@ -3191,7 +3203,7 @@
       <c r="K6" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="95"/>
+      <c r="L6" s="97"/>
       <c r="M6" s="72">
         <v>7.1400000000000005E-2</v>
       </c>
@@ -3204,7 +3216,7 @@
       <c r="P6" s="72">
         <v>0.16400000000000001</v>
       </c>
-      <c r="Q6" s="95"/>
+      <c r="Q6" s="97"/>
       <c r="R6" s="71">
         <v>116</v>
       </c>
@@ -3239,7 +3251,7 @@
       <c r="K7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="95"/>
+      <c r="L7" s="97"/>
       <c r="M7" s="75">
         <v>4.5789</v>
       </c>
@@ -3252,7 +3264,7 @@
       <c r="P7" s="75">
         <v>0.2122</v>
       </c>
-      <c r="Q7" s="95"/>
+      <c r="Q7" s="97"/>
       <c r="R7" s="6">
         <v>120</v>
       </c>
@@ -3287,7 +3299,7 @@
       <c r="K8" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="95"/>
+      <c r="L8" s="97"/>
       <c r="M8" s="72">
         <v>6.4744999999999999</v>
       </c>
@@ -3300,7 +3312,7 @@
       <c r="P8" s="72">
         <v>0.30930000000000002</v>
       </c>
-      <c r="Q8" s="95"/>
+      <c r="Q8" s="97"/>
       <c r="R8" s="71">
         <v>116</v>
       </c>
@@ -3335,7 +3347,7 @@
       <c r="K9" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L9" s="95"/>
+      <c r="L9" s="97"/>
       <c r="M9" s="72">
         <v>8.9992000000000001</v>
       </c>
@@ -3348,7 +3360,7 @@
       <c r="P9" s="72">
         <v>0.46489999999999998</v>
       </c>
-      <c r="Q9" s="95"/>
+      <c r="Q9" s="97"/>
       <c r="R9" s="71">
         <v>131</v>
       </c>
@@ -3383,7 +3395,7 @@
       <c r="K10" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="95"/>
+      <c r="L10" s="97"/>
       <c r="M10" s="72">
         <v>4.3776000000000002</v>
       </c>
@@ -3396,7 +3408,7 @@
       <c r="P10" s="72">
         <v>0.25719999999999998</v>
       </c>
-      <c r="Q10" s="95"/>
+      <c r="Q10" s="97"/>
       <c r="R10" s="71">
         <v>179</v>
       </c>
@@ -3431,7 +3443,7 @@
       <c r="K11" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="95"/>
+      <c r="L11" s="97"/>
       <c r="M11" s="72">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -3444,7 +3456,7 @@
       <c r="P11" s="72">
         <v>0.26069999999999999</v>
       </c>
-      <c r="Q11" s="95"/>
+      <c r="Q11" s="97"/>
       <c r="R11" s="71">
         <v>182</v>
       </c>
@@ -3479,7 +3491,7 @@
       <c r="K12" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="95"/>
+      <c r="L12" s="97"/>
       <c r="M12" s="72">
         <v>3.5999999999999999E-3</v>
       </c>
@@ -3492,7 +3504,7 @@
       <c r="P12" s="72">
         <v>0.39300000000000002</v>
       </c>
-      <c r="Q12" s="95"/>
+      <c r="Q12" s="97"/>
       <c r="R12" s="71">
         <v>89</v>
       </c>
@@ -3529,7 +3541,7 @@
       <c r="K13" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L13" s="95"/>
+      <c r="L13" s="97"/>
       <c r="M13" s="72">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -3542,7 +3554,7 @@
       <c r="P13" s="72">
         <v>0.41399999999999998</v>
       </c>
-      <c r="Q13" s="95"/>
+      <c r="Q13" s="97"/>
       <c r="R13" s="71">
         <v>44</v>
       </c>
@@ -3577,7 +3589,7 @@
       <c r="K14" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L14" s="95"/>
+      <c r="L14" s="97"/>
       <c r="M14" s="72">
         <v>1.1584000000000001</v>
       </c>
@@ -3590,7 +3602,7 @@
       <c r="P14" s="72">
         <v>0.1976</v>
       </c>
-      <c r="Q14" s="95"/>
+      <c r="Q14" s="97"/>
       <c r="R14" s="71">
         <v>305</v>
       </c>
@@ -3624,7 +3636,7 @@
       <c r="K15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L15" s="95"/>
+      <c r="L15" s="97"/>
       <c r="M15" s="75">
         <v>0.17349999999999999</v>
       </c>
@@ -3637,7 +3649,7 @@
       <c r="P15" s="75">
         <v>0.19939999999999999</v>
       </c>
-      <c r="Q15" s="95"/>
+      <c r="Q15" s="97"/>
       <c r="R15" s="6">
         <v>118</v>
       </c>
@@ -3671,7 +3683,7 @@
       <c r="K16" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L16" s="95"/>
+      <c r="L16" s="97"/>
       <c r="M16" s="72">
         <v>8.2579999999999991</v>
       </c>
@@ -3684,7 +3696,7 @@
       <c r="P16" s="72">
         <v>0.47870000000000001</v>
       </c>
-      <c r="Q16" s="95"/>
+      <c r="Q16" s="97"/>
       <c r="R16" s="71">
         <v>127</v>
       </c>
@@ -3714,7 +3726,7 @@
       <c r="K17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L17" s="95"/>
+      <c r="L17" s="97"/>
       <c r="M17" s="75">
         <v>3.5000000000000001E-3</v>
       </c>
@@ -3727,7 +3739,7 @@
       <c r="P17" s="75">
         <v>0.1825</v>
       </c>
-      <c r="Q17" s="95"/>
+      <c r="Q17" s="97"/>
       <c r="R17" s="6">
         <v>132</v>
       </c>
@@ -3744,12 +3756,12 @@
       <c r="I18" s="79"/>
       <c r="J18" s="79"/>
       <c r="K18" s="79"/>
-      <c r="L18" s="95"/>
+      <c r="L18" s="97"/>
       <c r="M18" s="80"/>
       <c r="N18" s="80"/>
       <c r="O18" s="80"/>
       <c r="P18" s="80"/>
-      <c r="Q18" s="95"/>
+      <c r="Q18" s="97"/>
       <c r="R18" s="81"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
@@ -3777,7 +3789,7 @@
       <c r="K19" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="L19" s="95"/>
+      <c r="L19" s="97"/>
       <c r="M19" s="85">
         <v>1.8E-3</v>
       </c>
@@ -3790,7 +3802,7 @@
       <c r="P19" s="85">
         <v>0.3236</v>
       </c>
-      <c r="Q19" s="95"/>
+      <c r="Q19" s="97"/>
       <c r="R19" s="84">
         <v>117</v>
       </c>
@@ -3820,7 +3832,7 @@
       <c r="K20" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L20" s="94"/>
+      <c r="L20" s="96"/>
       <c r="M20" s="72">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -3833,7 +3845,7 @@
       <c r="P20" s="72">
         <v>0.34599999999999997</v>
       </c>
-      <c r="Q20" s="94"/>
+      <c r="Q20" s="96"/>
       <c r="R20" s="71">
         <v>77</v>
       </c>
@@ -3849,12 +3861,12 @@
       <c r="I21" s="71"/>
       <c r="J21" s="71"/>
       <c r="K21" s="71"/>
-      <c r="L21" s="95"/>
+      <c r="L21" s="97"/>
       <c r="M21" s="72"/>
       <c r="N21" s="72"/>
       <c r="O21" s="72"/>
       <c r="P21" s="72"/>
-      <c r="Q21" s="95"/>
+      <c r="Q21" s="97"/>
       <c r="R21" s="71"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
@@ -3868,12 +3880,12 @@
       <c r="I22" s="71"/>
       <c r="J22" s="71"/>
       <c r="K22" s="71"/>
-      <c r="L22" s="95"/>
+      <c r="L22" s="97"/>
       <c r="M22" s="72"/>
       <c r="N22" s="72"/>
       <c r="O22" s="72"/>
       <c r="P22" s="72"/>
-      <c r="Q22" s="95"/>
+      <c r="Q22" s="97"/>
       <c r="R22" s="71"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
@@ -3887,12 +3899,12 @@
       <c r="I23" s="71"/>
       <c r="J23" s="71"/>
       <c r="K23" s="71"/>
-      <c r="L23" s="95"/>
+      <c r="L23" s="97"/>
       <c r="M23" s="72"/>
       <c r="N23" s="72"/>
       <c r="O23" s="72"/>
       <c r="P23" s="72"/>
-      <c r="Q23" s="95"/>
+      <c r="Q23" s="97"/>
       <c r="R23" s="71"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
@@ -3906,12 +3918,12 @@
       <c r="I24" s="71"/>
       <c r="J24" s="71"/>
       <c r="K24" s="71"/>
-      <c r="L24" s="95"/>
+      <c r="L24" s="97"/>
       <c r="M24" s="72"/>
       <c r="N24" s="72"/>
       <c r="O24" s="72"/>
       <c r="P24" s="72"/>
-      <c r="Q24" s="95"/>
+      <c r="Q24" s="97"/>
       <c r="R24" s="71"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
@@ -3925,12 +3937,12 @@
       <c r="I25" s="71"/>
       <c r="J25" s="71"/>
       <c r="K25" s="71"/>
-      <c r="L25" s="95"/>
+      <c r="L25" s="97"/>
       <c r="M25" s="72"/>
       <c r="N25" s="72"/>
       <c r="O25" s="72"/>
       <c r="P25" s="72"/>
-      <c r="Q25" s="95"/>
+      <c r="Q25" s="97"/>
       <c r="R25" s="71"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
@@ -3944,12 +3956,12 @@
       <c r="I26" s="71"/>
       <c r="J26" s="71"/>
       <c r="K26" s="71"/>
-      <c r="L26" s="95"/>
+      <c r="L26" s="97"/>
       <c r="M26" s="72"/>
       <c r="N26" s="72"/>
       <c r="O26" s="72"/>
       <c r="P26" s="72"/>
-      <c r="Q26" s="95"/>
+      <c r="Q26" s="97"/>
       <c r="R26" s="71"/>
     </row>
   </sheetData>
@@ -3972,8 +3984,8 @@
   </sheetPr>
   <dimension ref="B3:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3984,54 +3996,54 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="89" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="96" t="s">
+      <c r="C3" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="96" t="s">
+      <c r="D3" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="96" t="s">
+      <c r="E3" s="88" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="96" t="s">
+      <c r="F3" s="88" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="96" t="s">
+      <c r="G3" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="96" t="s">
+      <c r="H3" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="I3" s="96" t="s">
+      <c r="I3" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="J3" s="96" t="s">
+      <c r="J3" s="88" t="s">
         <v>71</v>
       </c>
-      <c r="K3" s="96" t="s">
+      <c r="K3" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="96" t="s">
+      <c r="L3" s="88" t="s">
         <v>11</v>
       </c>
       <c r="M3" s="86"/>
-      <c r="N3" s="96" t="s">
+      <c r="N3" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="96" t="s">
+      <c r="O3" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="96" t="s">
+      <c r="P3" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="96" t="s">
+      <c r="Q3" s="88" t="s">
         <v>10</v>
       </c>
       <c r="R3" s="86"/>
-      <c r="S3" s="96" t="s">
+      <c r="S3" s="88" t="s">
         <v>56</v>
       </c>
     </row>
@@ -4128,77 +4140,167 @@
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
+      <c r="B6" s="71" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="71" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="71">
+        <v>50</v>
+      </c>
+      <c r="E6" s="71" t="s">
+        <v>62</v>
+      </c>
       <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
+      <c r="G6" s="71">
+        <v>1E-4</v>
+      </c>
+      <c r="H6" s="71">
+        <v>200</v>
+      </c>
+      <c r="I6" s="71">
+        <v>4</v>
+      </c>
       <c r="J6" s="71"/>
       <c r="K6" s="71"/>
-      <c r="L6" s="71"/>
+      <c r="L6" s="71" t="s">
+        <v>6</v>
+      </c>
       <c r="M6" s="87"/>
-      <c r="N6" s="72"/>
-      <c r="O6" s="72"/>
-      <c r="P6" s="72"/>
-      <c r="Q6" s="72"/>
+      <c r="N6" s="72">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="O6" s="72">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="P6" s="72">
+        <v>0.11459999999999999</v>
+      </c>
+      <c r="Q6" s="72">
+        <v>0.29720000000000002</v>
+      </c>
       <c r="R6" s="87"/>
-      <c r="S6" s="71"/>
+      <c r="S6" s="71">
+        <v>87</v>
+      </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
+      <c r="C7" s="71" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="71">
+        <v>50</v>
+      </c>
+      <c r="E7" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="71" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="71">
+        <v>1E-4</v>
+      </c>
+      <c r="H7" s="71">
+        <v>200</v>
+      </c>
+      <c r="I7" s="71">
+        <v>4</v>
+      </c>
       <c r="J7" s="71"/>
       <c r="K7" s="71"/>
-      <c r="L7" s="71"/>
+      <c r="L7" s="71" t="s">
+        <v>6</v>
+      </c>
       <c r="M7" s="87"/>
-      <c r="N7" s="72"/>
-      <c r="O7" s="72"/>
-      <c r="P7" s="72"/>
-      <c r="Q7" s="72"/>
+      <c r="N7" s="72">
+        <v>0.15970000000000001</v>
+      </c>
+      <c r="O7" s="72">
+        <v>9.7000000000000003E-3</v>
+      </c>
+      <c r="P7" s="72">
+        <v>4.6406000000000001</v>
+      </c>
+      <c r="Q7" s="72">
+        <v>0.29559999999999997</v>
+      </c>
       <c r="R7" s="87"/>
-      <c r="S7" s="71"/>
+      <c r="S7" s="71">
+        <v>91</v>
+      </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
+      <c r="C8" s="71" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="71">
+        <v>50</v>
+      </c>
+      <c r="E8" s="71" t="s">
+        <v>61</v>
+      </c>
       <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="71"/>
+      <c r="G8" s="71">
+        <v>0.01</v>
+      </c>
+      <c r="H8" s="71">
+        <v>200</v>
+      </c>
+      <c r="I8" s="71">
+        <v>16</v>
+      </c>
       <c r="J8" s="71"/>
       <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
+      <c r="L8" s="71" t="s">
+        <v>6</v>
+      </c>
       <c r="M8" s="87"/>
-      <c r="N8" s="72"/>
-      <c r="O8" s="72"/>
-      <c r="P8" s="72"/>
-      <c r="Q8" s="72"/>
+      <c r="N8" s="72">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="O8" s="72">
+        <v>1.72E-2</v>
+      </c>
+      <c r="P8" s="72">
+        <v>0.1318</v>
+      </c>
+      <c r="Q8" s="72">
+        <v>0.34460000000000002</v>
+      </c>
       <c r="R8" s="87"/>
-      <c r="S8" s="71"/>
+      <c r="S8" s="71">
+        <v>82</v>
+      </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
+      <c r="C9" s="71" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="71">
+        <v>50</v>
+      </c>
+      <c r="E9" s="71" t="s">
+        <v>61</v>
+      </c>
       <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="71"/>
+      <c r="G9" s="71">
+        <v>0.01</v>
+      </c>
+      <c r="H9" s="71">
+        <v>300</v>
+      </c>
+      <c r="I9" s="71">
+        <v>32</v>
+      </c>
       <c r="J9" s="71"/>
       <c r="K9" s="71"/>
-      <c r="L9" s="71"/>
+      <c r="L9" s="71" t="s">
+        <v>18</v>
+      </c>
       <c r="M9" s="87"/>
       <c r="N9" s="72"/>
       <c r="O9" s="72"/>

</xml_diff>

<commit_message>
Add - guardado de modelos de testing y modelo y gráfica VSCd de 1_HEMU1
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\MemoriaCodigoFuentev3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A70DCF-119E-4272-9C00-68D9D08C6B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE621104-714D-4C8F-ADFA-4A28E673F14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3135" yWindow="7710" windowWidth="21600" windowHeight="7695" activeTab="2" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
+    <workbookView xWindow="2040" yWindow="7290" windowWidth="23310" windowHeight="7695" activeTab="3" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
   <sheets>
     <sheet name="full_signals - without decay" sheetId="1" r:id="rId1"/>
     <sheet name="full_signals - with decay" sheetId="2" r:id="rId2"/>
     <sheet name="modelos por sujeto sano" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="98">
   <si>
     <t>MODELO U-NET: FULL SIGNALS</t>
   </si>
@@ -320,6 +321,39 @@
   <si>
     <t>unet_model_vscdv6.keras</t>
   </si>
+  <si>
+    <t>unet_model_vscdv7.keras</t>
+  </si>
+  <si>
+    <t>unet_model_vscdv8.keras</t>
+  </si>
+  <si>
+    <t>mejor error</t>
+  </si>
+  <si>
+    <t>mejor error con decaimiento de LR</t>
+  </si>
+  <si>
+    <t>unet_model_vscdv9.keras</t>
+  </si>
+  <si>
+    <t>curvas de NMSE sin convergencia</t>
+  </si>
+  <si>
+    <t>unet_model_vscdv10.keras</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>9.3988e-0.4</t>
+  </si>
+  <si>
+    <t>unet_model_vscd_derecho.keras</t>
+  </si>
+  <si>
+    <t>unet_model_vsci_izquierdo.keras</t>
+  </si>
 </sst>
 </file>
 
@@ -329,7 +363,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,8 +434,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -516,6 +557,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -577,7 +624,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -860,6 +907,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1205,7 +1258,7 @@
   </sheetPr>
   <dimension ref="B2:R54"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="A28" sqref="A28:XFD32"/>
     </sheetView>
   </sheetViews>
@@ -3101,7 +3154,7 @@
   <dimension ref="B3:S26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
@@ -3982,10 +4035,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="B3:S13"/>
+  <dimension ref="B3:W13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3993,9 +4046,11 @@
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
     <col min="2" max="2" width="59.140625" customWidth="1"/>
     <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="20" max="20" width="31.85546875" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:23" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="89" t="s">
         <v>81</v>
       </c>
@@ -4047,7 +4102,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B4" s="71" t="s">
         <v>82</v>
       </c>
@@ -4093,7 +4148,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B5" s="71" t="s">
         <v>82</v>
       </c>
@@ -4139,53 +4194,56 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" s="71" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="71" t="s">
+      <c r="C6" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="71">
+      <c r="D6" s="6">
         <v>50</v>
       </c>
-      <c r="E6" s="71" t="s">
+      <c r="E6" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71">
-        <v>1E-4</v>
-      </c>
-      <c r="H6" s="71">
+      <c r="F6" s="6"/>
+      <c r="G6" s="6">
+        <v>1E-4</v>
+      </c>
+      <c r="H6" s="6">
         <v>200</v>
       </c>
-      <c r="I6" s="71">
+      <c r="I6" s="6">
         <v>4</v>
       </c>
-      <c r="J6" s="71"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="71" t="s">
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="M6" s="87"/>
-      <c r="N6" s="72">
+      <c r="N6" s="75">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="O6" s="72">
+      <c r="O6" s="75">
         <v>4.1999999999999997E-3</v>
       </c>
-      <c r="P6" s="72">
+      <c r="P6" s="75">
         <v>0.11459999999999999</v>
       </c>
-      <c r="Q6" s="72">
+      <c r="Q6" s="75">
         <v>0.29720000000000002</v>
       </c>
       <c r="R6" s="87"/>
-      <c r="S6" s="71">
+      <c r="S6" s="6">
         <v>87</v>
       </c>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T6" s="99" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B7" s="71"/>
       <c r="C7" s="71" t="s">
         <v>84</v>
@@ -4231,7 +4289,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B8" s="71"/>
       <c r="C8" s="71" t="s">
         <v>85</v>
@@ -4275,7 +4333,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B9" s="71"/>
       <c r="C9" s="71" t="s">
         <v>86</v>
@@ -4302,92 +4360,382 @@
         <v>18</v>
       </c>
       <c r="M9" s="87"/>
-      <c r="N9" s="72"/>
-      <c r="O9" s="72"/>
-      <c r="P9" s="72"/>
-      <c r="Q9" s="72"/>
+      <c r="N9" s="72">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="O9" s="72">
+        <v>1.8200000000000001E-2</v>
+      </c>
+      <c r="P9" s="72">
+        <v>0.1265</v>
+      </c>
+      <c r="Q9" s="72">
+        <v>0.33079999999999998</v>
+      </c>
       <c r="R9" s="87"/>
-      <c r="S9" s="71"/>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S9" s="71">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
+      <c r="C10" s="71" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="71">
+        <v>50</v>
+      </c>
+      <c r="E10" s="71" t="s">
+        <v>62</v>
+      </c>
       <c r="F10" s="71"/>
-      <c r="G10" s="71"/>
-      <c r="H10" s="71"/>
-      <c r="I10" s="71"/>
+      <c r="G10" s="71">
+        <v>1E-4</v>
+      </c>
+      <c r="H10" s="71">
+        <v>250</v>
+      </c>
+      <c r="I10" s="71">
+        <v>4</v>
+      </c>
       <c r="J10" s="71"/>
       <c r="K10" s="71"/>
-      <c r="L10" s="71"/>
+      <c r="L10" s="71" t="s">
+        <v>6</v>
+      </c>
       <c r="M10" s="87"/>
-      <c r="N10" s="72"/>
-      <c r="O10" s="72"/>
-      <c r="P10" s="72"/>
-      <c r="Q10" s="72"/>
+      <c r="N10" s="72">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="O10" s="72">
+        <v>8.8999999999999999E-3</v>
+      </c>
+      <c r="P10" s="72">
+        <v>0.1157</v>
+      </c>
+      <c r="Q10" s="72">
+        <v>0.29830000000000001</v>
+      </c>
       <c r="R10" s="87"/>
-      <c r="S10" s="71"/>
-    </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S10" s="71">
+        <v>111</v>
+      </c>
+      <c r="T10" s="100"/>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B11" s="71"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
+      <c r="C11" s="71" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="71">
+        <v>50</v>
+      </c>
+      <c r="E11" s="71" t="s">
+        <v>62</v>
+      </c>
       <c r="F11" s="71"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71"/>
+      <c r="G11" s="71">
+        <v>1E-4</v>
+      </c>
+      <c r="H11" s="71">
+        <v>200</v>
+      </c>
+      <c r="I11" s="71">
+        <v>4</v>
+      </c>
       <c r="J11" s="71"/>
-      <c r="K11" s="71"/>
-      <c r="L11" s="71"/>
+      <c r="K11" s="98">
+        <f>(D11/I11)*H11</f>
+        <v>2500</v>
+      </c>
+      <c r="L11" s="71" t="s">
+        <v>6</v>
+      </c>
       <c r="M11" s="87"/>
-      <c r="N11" s="72"/>
-      <c r="O11" s="72"/>
-      <c r="P11" s="72"/>
-      <c r="Q11" s="72"/>
+      <c r="N11" s="72">
+        <v>7.5700000000000003E-2</v>
+      </c>
+      <c r="O11" s="72">
+        <v>0.18679999999999999</v>
+      </c>
+      <c r="P11" s="72">
+        <v>0.11509999999999999</v>
+      </c>
+      <c r="Q11" s="72">
+        <v>0.29749999999999999</v>
+      </c>
       <c r="R11" s="87"/>
-      <c r="S11" s="71"/>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S11" s="71">
+        <v>86</v>
+      </c>
+      <c r="T11" s="99" t="s">
+        <v>90</v>
+      </c>
+      <c r="U11" s="101" t="s">
+        <v>92</v>
+      </c>
+      <c r="V11" s="101"/>
+      <c r="W11" s="101"/>
+    </row>
+    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B12" s="71"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
+      <c r="C12" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="71">
+        <v>50</v>
+      </c>
+      <c r="E12" s="71" t="s">
+        <v>62</v>
+      </c>
       <c r="F12" s="71"/>
-      <c r="G12" s="71"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="71"/>
+      <c r="G12" s="71">
+        <v>1E-4</v>
+      </c>
+      <c r="H12" s="71">
+        <v>400</v>
+      </c>
+      <c r="I12" s="71">
+        <v>4</v>
+      </c>
       <c r="J12" s="71"/>
-      <c r="K12" s="71"/>
-      <c r="L12" s="71"/>
+      <c r="K12" s="98">
+        <f>(D12/I12)*H12</f>
+        <v>5000</v>
+      </c>
+      <c r="L12" s="71" t="s">
+        <v>6</v>
+      </c>
       <c r="M12" s="87"/>
-      <c r="N12" s="72"/>
-      <c r="O12" s="72"/>
-      <c r="P12" s="72"/>
-      <c r="Q12" s="72"/>
+      <c r="N12" s="72">
+        <v>2.4799999999999999E-2</v>
+      </c>
+      <c r="O12" s="72">
+        <v>6.1600000000000002E-2</v>
+      </c>
+      <c r="P12" s="72">
+        <v>0.13619999999999999</v>
+      </c>
+      <c r="Q12" s="72">
+        <v>0.3528</v>
+      </c>
       <c r="R12" s="87"/>
-      <c r="S12" s="71"/>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S12" s="71">
+        <v>174</v>
+      </c>
+      <c r="T12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
+      <c r="C13" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="71">
+        <v>50</v>
+      </c>
+      <c r="E13" s="71" t="s">
+        <v>61</v>
+      </c>
       <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="71"/>
+      <c r="G13" s="71">
+        <v>1E-4</v>
+      </c>
+      <c r="H13" s="71">
+        <v>400</v>
+      </c>
+      <c r="I13" s="71">
+        <v>8</v>
+      </c>
       <c r="J13" s="71"/>
-      <c r="K13" s="71"/>
-      <c r="L13" s="71"/>
+      <c r="K13" s="98">
+        <f>(D13/I13)*H13</f>
+        <v>2500</v>
+      </c>
+      <c r="L13" s="71" t="s">
+        <v>6</v>
+      </c>
       <c r="M13" s="87"/>
-      <c r="N13" s="72"/>
-      <c r="O13" s="72"/>
-      <c r="P13" s="72"/>
-      <c r="Q13" s="72"/>
+      <c r="N13" s="72" t="s">
+        <v>95</v>
+      </c>
+      <c r="O13" s="72">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="P13" s="72">
+        <v>0.12670000000000001</v>
+      </c>
+      <c r="Q13" s="72">
+        <v>0.32279999999999998</v>
+      </c>
       <c r="R13" s="87"/>
-      <c r="S13" s="71"/>
+      <c r="S13" s="71">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71B16EA-A98B-40B8-9C49-FBDC385B3C23}">
+  <dimension ref="C3:U5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="0.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="38.42578125" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" customWidth="1"/>
+    <col min="12" max="12" width="5.5703125" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" customWidth="1"/>
+    <col min="15" max="15" width="4.28515625" customWidth="1"/>
+    <col min="20" max="20" width="4.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="D3" s="89" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="88" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="88" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="88" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="88" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="88" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="88" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" s="88" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" s="88" t="s">
+        <v>71</v>
+      </c>
+      <c r="M3" s="88" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="86"/>
+      <c r="P3" s="88" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="88" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3" s="88" t="s">
+        <v>9</v>
+      </c>
+      <c r="S3" s="88" t="s">
+        <v>10</v>
+      </c>
+      <c r="T3" s="86"/>
+      <c r="U3" s="88" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D4" s="71" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="71">
+        <v>50</v>
+      </c>
+      <c r="G4" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71">
+        <v>1E-4</v>
+      </c>
+      <c r="J4" s="71">
+        <v>200</v>
+      </c>
+      <c r="K4" s="71">
+        <v>8</v>
+      </c>
+      <c r="L4" s="71"/>
+      <c r="M4" s="71"/>
+      <c r="N4" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4" s="87"/>
+      <c r="P4" s="72">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="Q4" s="72">
+        <v>1.23E-2</v>
+      </c>
+      <c r="R4" s="72">
+        <v>0.12690000000000001</v>
+      </c>
+      <c r="S4" s="72">
+        <v>0.3291</v>
+      </c>
+      <c r="T4" s="87"/>
+      <c r="U4" s="71">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D5" s="71" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="71" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="71">
+        <v>50</v>
+      </c>
+      <c r="G5" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71">
+        <v>1E-4</v>
+      </c>
+      <c r="J5" s="71">
+        <v>300</v>
+      </c>
+      <c r="K5" s="71">
+        <v>8</v>
+      </c>
+      <c r="L5" s="71"/>
+      <c r="M5" s="71"/>
+      <c r="N5" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5" s="87"/>
+      <c r="P5" s="72"/>
+      <c r="Q5" s="72"/>
+      <c r="R5" s="72"/>
+      <c r="S5" s="72"/>
+      <c r="T5" s="87"/>
+      <c r="U5" s="71"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add - se guardan modelos se 2_DAOC
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\MemoriaCodigoFuentev3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE621104-714D-4C8F-ADFA-4A28E673F14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318123CB-65A2-467D-B874-AAAFDAD5E800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="7290" windowWidth="23310" windowHeight="7695" activeTab="3" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
+    <workbookView xWindow="4200" yWindow="5790" windowWidth="23310" windowHeight="7695" activeTab="3" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
   <sheets>
     <sheet name="full_signals - without decay" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="102">
   <si>
     <t>MODELO U-NET: FULL SIGNALS</t>
   </si>
@@ -353,6 +353,18 @@
   </si>
   <si>
     <t>unet_model_vsci_izquierdo.keras</t>
+  </si>
+  <si>
+    <t>2_DAOC</t>
+  </si>
+  <si>
+    <t>3_DASI</t>
+  </si>
+  <si>
+    <t>80/21</t>
+  </si>
+  <si>
+    <t>80/22</t>
   </si>
 </sst>
 </file>
@@ -442,7 +454,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -563,8 +575,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -620,11 +650,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -883,6 +926,11 @@
     <xf numFmtId="0" fontId="9" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -907,12 +955,77 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="21" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="21" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="22" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="23" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1280,24 +1393,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="94"/>
     </row>
     <row r="4" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -2086,10 +2199,10 @@
       <c r="P23" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q23" s="93" t="s">
+      <c r="Q23" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="R23" s="94"/>
+      <c r="R23" s="97"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
@@ -2129,8 +2242,8 @@
       <c r="P24" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q24" s="95"/>
-      <c r="R24" s="94"/>
+      <c r="Q24" s="98"/>
+      <c r="R24" s="97"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
@@ -2170,8 +2283,8 @@
       <c r="P25" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q25" s="95"/>
-      <c r="R25" s="94"/>
+      <c r="Q25" s="98"/>
+      <c r="R25" s="97"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="18" t="s">
@@ -2211,8 +2324,8 @@
       <c r="P26" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q26" s="95"/>
-      <c r="R26" s="94"/>
+      <c r="Q26" s="98"/>
+      <c r="R26" s="97"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="29" t="s">
@@ -2252,8 +2365,8 @@
       <c r="P27" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q27" s="95"/>
-      <c r="R27" s="94"/>
+      <c r="Q27" s="98"/>
+      <c r="R27" s="97"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
@@ -2293,8 +2406,8 @@
       <c r="P28" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q28" s="95"/>
-      <c r="R28" s="94"/>
+      <c r="Q28" s="98"/>
+      <c r="R28" s="97"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
@@ -2334,8 +2447,8 @@
       <c r="P29" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="95"/>
-      <c r="R29" s="94"/>
+      <c r="Q29" s="98"/>
+      <c r="R29" s="97"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="18" t="s">
@@ -2375,8 +2488,8 @@
       <c r="P30" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q30" s="95"/>
-      <c r="R30" s="94"/>
+      <c r="Q30" s="98"/>
+      <c r="R30" s="97"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
@@ -2416,8 +2529,8 @@
       <c r="P31" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q31" s="95"/>
-      <c r="R31" s="94"/>
+      <c r="Q31" s="98"/>
+      <c r="R31" s="97"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="29" t="s">
@@ -2457,8 +2570,8 @@
       <c r="P32" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q32" s="95"/>
-      <c r="R32" s="94"/>
+      <c r="Q32" s="98"/>
+      <c r="R32" s="97"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
@@ -2498,8 +2611,8 @@
       <c r="P33" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q33" s="95"/>
-      <c r="R33" s="94"/>
+      <c r="Q33" s="98"/>
+      <c r="R33" s="97"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
@@ -2539,8 +2652,8 @@
       <c r="P34" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q34" s="95"/>
-      <c r="R34" s="94"/>
+      <c r="Q34" s="98"/>
+      <c r="R34" s="97"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="18" t="s">
@@ -2580,8 +2693,8 @@
       <c r="P35" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q35" s="95"/>
-      <c r="R35" s="94"/>
+      <c r="Q35" s="98"/>
+      <c r="R35" s="97"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="18" t="s">
@@ -2621,8 +2734,8 @@
       <c r="P36" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q36" s="95"/>
-      <c r="R36" s="94"/>
+      <c r="Q36" s="98"/>
+      <c r="R36" s="97"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="29" t="s">
@@ -2662,21 +2775,21 @@
       <c r="P37" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q37" s="95"/>
-      <c r="R37" s="94"/>
+      <c r="Q37" s="98"/>
+      <c r="R37" s="97"/>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B39" s="92" t="s">
+      <c r="B39" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="92"/>
-      <c r="D39" s="92"/>
-      <c r="E39" s="92"/>
-      <c r="F39" s="92"/>
-      <c r="G39" s="92"/>
-      <c r="H39" s="92"/>
-      <c r="I39" s="92"/>
-      <c r="J39" s="92"/>
+      <c r="C39" s="95"/>
+      <c r="D39" s="95"/>
+      <c r="E39" s="95"/>
+      <c r="F39" s="95"/>
+      <c r="G39" s="95"/>
+      <c r="H39" s="95"/>
+      <c r="I39" s="95"/>
+      <c r="J39" s="95"/>
     </row>
     <row r="40" spans="2:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="49" t="s">
@@ -3174,10 +3287,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="90"/>
+      <c r="C3" s="93"/>
     </row>
     <row r="5" spans="2:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="69" t="s">
@@ -3210,7 +3323,7 @@
       <c r="K5" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="96"/>
+      <c r="L5" s="99"/>
       <c r="M5" s="69" t="s">
         <v>7</v>
       </c>
@@ -3223,7 +3336,7 @@
       <c r="P5" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" s="96"/>
+      <c r="Q5" s="99"/>
       <c r="R5" s="69" t="s">
         <v>56</v>
       </c>
@@ -3256,7 +3369,7 @@
       <c r="K6" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="97"/>
+      <c r="L6" s="100"/>
       <c r="M6" s="72">
         <v>7.1400000000000005E-2</v>
       </c>
@@ -3269,7 +3382,7 @@
       <c r="P6" s="72">
         <v>0.16400000000000001</v>
       </c>
-      <c r="Q6" s="97"/>
+      <c r="Q6" s="100"/>
       <c r="R6" s="71">
         <v>116</v>
       </c>
@@ -3304,7 +3417,7 @@
       <c r="K7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="97"/>
+      <c r="L7" s="100"/>
       <c r="M7" s="75">
         <v>4.5789</v>
       </c>
@@ -3317,7 +3430,7 @@
       <c r="P7" s="75">
         <v>0.2122</v>
       </c>
-      <c r="Q7" s="97"/>
+      <c r="Q7" s="100"/>
       <c r="R7" s="6">
         <v>120</v>
       </c>
@@ -3352,7 +3465,7 @@
       <c r="K8" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="97"/>
+      <c r="L8" s="100"/>
       <c r="M8" s="72">
         <v>6.4744999999999999</v>
       </c>
@@ -3365,7 +3478,7 @@
       <c r="P8" s="72">
         <v>0.30930000000000002</v>
       </c>
-      <c r="Q8" s="97"/>
+      <c r="Q8" s="100"/>
       <c r="R8" s="71">
         <v>116</v>
       </c>
@@ -3400,7 +3513,7 @@
       <c r="K9" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L9" s="97"/>
+      <c r="L9" s="100"/>
       <c r="M9" s="72">
         <v>8.9992000000000001</v>
       </c>
@@ -3413,7 +3526,7 @@
       <c r="P9" s="72">
         <v>0.46489999999999998</v>
       </c>
-      <c r="Q9" s="97"/>
+      <c r="Q9" s="100"/>
       <c r="R9" s="71">
         <v>131</v>
       </c>
@@ -3448,7 +3561,7 @@
       <c r="K10" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="97"/>
+      <c r="L10" s="100"/>
       <c r="M10" s="72">
         <v>4.3776000000000002</v>
       </c>
@@ -3461,7 +3574,7 @@
       <c r="P10" s="72">
         <v>0.25719999999999998</v>
       </c>
-      <c r="Q10" s="97"/>
+      <c r="Q10" s="100"/>
       <c r="R10" s="71">
         <v>179</v>
       </c>
@@ -3496,7 +3609,7 @@
       <c r="K11" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="97"/>
+      <c r="L11" s="100"/>
       <c r="M11" s="72">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -3509,7 +3622,7 @@
       <c r="P11" s="72">
         <v>0.26069999999999999</v>
       </c>
-      <c r="Q11" s="97"/>
+      <c r="Q11" s="100"/>
       <c r="R11" s="71">
         <v>182</v>
       </c>
@@ -3544,7 +3657,7 @@
       <c r="K12" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="97"/>
+      <c r="L12" s="100"/>
       <c r="M12" s="72">
         <v>3.5999999999999999E-3</v>
       </c>
@@ -3557,7 +3670,7 @@
       <c r="P12" s="72">
         <v>0.39300000000000002</v>
       </c>
-      <c r="Q12" s="97"/>
+      <c r="Q12" s="100"/>
       <c r="R12" s="71">
         <v>89</v>
       </c>
@@ -3594,7 +3707,7 @@
       <c r="K13" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L13" s="97"/>
+      <c r="L13" s="100"/>
       <c r="M13" s="72">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -3607,7 +3720,7 @@
       <c r="P13" s="72">
         <v>0.41399999999999998</v>
       </c>
-      <c r="Q13" s="97"/>
+      <c r="Q13" s="100"/>
       <c r="R13" s="71">
         <v>44</v>
       </c>
@@ -3642,7 +3755,7 @@
       <c r="K14" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L14" s="97"/>
+      <c r="L14" s="100"/>
       <c r="M14" s="72">
         <v>1.1584000000000001</v>
       </c>
@@ -3655,7 +3768,7 @@
       <c r="P14" s="72">
         <v>0.1976</v>
       </c>
-      <c r="Q14" s="97"/>
+      <c r="Q14" s="100"/>
       <c r="R14" s="71">
         <v>305</v>
       </c>
@@ -3689,7 +3802,7 @@
       <c r="K15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L15" s="97"/>
+      <c r="L15" s="100"/>
       <c r="M15" s="75">
         <v>0.17349999999999999</v>
       </c>
@@ -3702,7 +3815,7 @@
       <c r="P15" s="75">
         <v>0.19939999999999999</v>
       </c>
-      <c r="Q15" s="97"/>
+      <c r="Q15" s="100"/>
       <c r="R15" s="6">
         <v>118</v>
       </c>
@@ -3736,7 +3849,7 @@
       <c r="K16" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L16" s="97"/>
+      <c r="L16" s="100"/>
       <c r="M16" s="72">
         <v>8.2579999999999991</v>
       </c>
@@ -3749,7 +3862,7 @@
       <c r="P16" s="72">
         <v>0.47870000000000001</v>
       </c>
-      <c r="Q16" s="97"/>
+      <c r="Q16" s="100"/>
       <c r="R16" s="71">
         <v>127</v>
       </c>
@@ -3779,7 +3892,7 @@
       <c r="K17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L17" s="97"/>
+      <c r="L17" s="100"/>
       <c r="M17" s="75">
         <v>3.5000000000000001E-3</v>
       </c>
@@ -3792,7 +3905,7 @@
       <c r="P17" s="75">
         <v>0.1825</v>
       </c>
-      <c r="Q17" s="97"/>
+      <c r="Q17" s="100"/>
       <c r="R17" s="6">
         <v>132</v>
       </c>
@@ -3809,12 +3922,12 @@
       <c r="I18" s="79"/>
       <c r="J18" s="79"/>
       <c r="K18" s="79"/>
-      <c r="L18" s="97"/>
+      <c r="L18" s="100"/>
       <c r="M18" s="80"/>
       <c r="N18" s="80"/>
       <c r="O18" s="80"/>
       <c r="P18" s="80"/>
-      <c r="Q18" s="97"/>
+      <c r="Q18" s="100"/>
       <c r="R18" s="81"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
@@ -3842,7 +3955,7 @@
       <c r="K19" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="L19" s="97"/>
+      <c r="L19" s="100"/>
       <c r="M19" s="85">
         <v>1.8E-3</v>
       </c>
@@ -3855,7 +3968,7 @@
       <c r="P19" s="85">
         <v>0.3236</v>
       </c>
-      <c r="Q19" s="97"/>
+      <c r="Q19" s="100"/>
       <c r="R19" s="84">
         <v>117</v>
       </c>
@@ -3885,7 +3998,7 @@
       <c r="K20" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L20" s="96"/>
+      <c r="L20" s="99"/>
       <c r="M20" s="72">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -3898,7 +4011,7 @@
       <c r="P20" s="72">
         <v>0.34599999999999997</v>
       </c>
-      <c r="Q20" s="96"/>
+      <c r="Q20" s="99"/>
       <c r="R20" s="71">
         <v>77</v>
       </c>
@@ -3914,12 +4027,12 @@
       <c r="I21" s="71"/>
       <c r="J21" s="71"/>
       <c r="K21" s="71"/>
-      <c r="L21" s="97"/>
+      <c r="L21" s="100"/>
       <c r="M21" s="72"/>
       <c r="N21" s="72"/>
       <c r="O21" s="72"/>
       <c r="P21" s="72"/>
-      <c r="Q21" s="97"/>
+      <c r="Q21" s="100"/>
       <c r="R21" s="71"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
@@ -3933,12 +4046,12 @@
       <c r="I22" s="71"/>
       <c r="J22" s="71"/>
       <c r="K22" s="71"/>
-      <c r="L22" s="97"/>
+      <c r="L22" s="100"/>
       <c r="M22" s="72"/>
       <c r="N22" s="72"/>
       <c r="O22" s="72"/>
       <c r="P22" s="72"/>
-      <c r="Q22" s="97"/>
+      <c r="Q22" s="100"/>
       <c r="R22" s="71"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
@@ -3952,12 +4065,12 @@
       <c r="I23" s="71"/>
       <c r="J23" s="71"/>
       <c r="K23" s="71"/>
-      <c r="L23" s="97"/>
+      <c r="L23" s="100"/>
       <c r="M23" s="72"/>
       <c r="N23" s="72"/>
       <c r="O23" s="72"/>
       <c r="P23" s="72"/>
-      <c r="Q23" s="97"/>
+      <c r="Q23" s="100"/>
       <c r="R23" s="71"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
@@ -3971,12 +4084,12 @@
       <c r="I24" s="71"/>
       <c r="J24" s="71"/>
       <c r="K24" s="71"/>
-      <c r="L24" s="97"/>
+      <c r="L24" s="100"/>
       <c r="M24" s="72"/>
       <c r="N24" s="72"/>
       <c r="O24" s="72"/>
       <c r="P24" s="72"/>
-      <c r="Q24" s="97"/>
+      <c r="Q24" s="100"/>
       <c r="R24" s="71"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
@@ -3990,12 +4103,12 @@
       <c r="I25" s="71"/>
       <c r="J25" s="71"/>
       <c r="K25" s="71"/>
-      <c r="L25" s="97"/>
+      <c r="L25" s="100"/>
       <c r="M25" s="72"/>
       <c r="N25" s="72"/>
       <c r="O25" s="72"/>
       <c r="P25" s="72"/>
-      <c r="Q25" s="97"/>
+      <c r="Q25" s="100"/>
       <c r="R25" s="71"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
@@ -4009,12 +4122,12 @@
       <c r="I26" s="71"/>
       <c r="J26" s="71"/>
       <c r="K26" s="71"/>
-      <c r="L26" s="97"/>
+      <c r="L26" s="100"/>
       <c r="M26" s="72"/>
       <c r="N26" s="72"/>
       <c r="O26" s="72"/>
       <c r="P26" s="72"/>
-      <c r="Q26" s="97"/>
+      <c r="Q26" s="100"/>
       <c r="R26" s="71"/>
     </row>
   </sheetData>
@@ -4239,7 +4352,7 @@
       <c r="S6" s="6">
         <v>87</v>
       </c>
-      <c r="T6" s="99" t="s">
+      <c r="T6" s="91" t="s">
         <v>89</v>
       </c>
     </row>
@@ -4420,7 +4533,6 @@
       <c r="S10" s="71">
         <v>111</v>
       </c>
-      <c r="T10" s="100"/>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B11" s="71"/>
@@ -4444,7 +4556,7 @@
         <v>4</v>
       </c>
       <c r="J11" s="71"/>
-      <c r="K11" s="98">
+      <c r="K11" s="90">
         <f>(D11/I11)*H11</f>
         <v>2500</v>
       </c>
@@ -4468,14 +4580,14 @@
       <c r="S11" s="71">
         <v>86</v>
       </c>
-      <c r="T11" s="99" t="s">
+      <c r="T11" s="91" t="s">
         <v>90</v>
       </c>
-      <c r="U11" s="101" t="s">
+      <c r="U11" s="92" t="s">
         <v>92</v>
       </c>
-      <c r="V11" s="101"/>
-      <c r="W11" s="101"/>
+      <c r="V11" s="92"/>
+      <c r="W11" s="92"/>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B12" s="71"/>
@@ -4499,7 +4611,7 @@
         <v>4</v>
       </c>
       <c r="J12" s="71"/>
-      <c r="K12" s="98">
+      <c r="K12" s="90">
         <f>(D12/I12)*H12</f>
         <v>5000</v>
       </c>
@@ -4549,7 +4661,7 @@
         <v>8</v>
       </c>
       <c r="J13" s="71"/>
-      <c r="K13" s="98">
+      <c r="K13" s="90">
         <f>(D13/I13)*H13</f>
         <v>2500</v>
       </c>
@@ -4581,10 +4693,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71B16EA-A98B-40B8-9C49-FBDC385B3C23}">
-  <dimension ref="C3:U5"/>
+  <dimension ref="D3:U18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3:O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4637,7 +4749,7 @@
       <c r="N3" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="86"/>
+      <c r="O3" s="99"/>
       <c r="P3" s="88" t="s">
         <v>7</v>
       </c>
@@ -4650,94 +4762,440 @@
       <c r="S3" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="T3" s="86"/>
+      <c r="T3" s="100"/>
       <c r="U3" s="88" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="4" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="71" t="s">
+      <c r="E4" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="F4" s="71">
+      <c r="F4" s="12">
         <v>50</v>
       </c>
-      <c r="G4" s="71" t="s">
+      <c r="G4" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71">
-        <v>1E-4</v>
-      </c>
-      <c r="J4" s="71">
+      <c r="H4" s="12"/>
+      <c r="I4" s="12">
+        <v>1E-4</v>
+      </c>
+      <c r="J4" s="12">
         <v>200</v>
       </c>
-      <c r="K4" s="71">
+      <c r="K4" s="12">
         <v>8</v>
       </c>
-      <c r="L4" s="71"/>
-      <c r="M4" s="71"/>
-      <c r="N4" s="71" t="s">
-        <v>6</v>
-      </c>
-      <c r="O4" s="87"/>
-      <c r="P4" s="72">
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4" s="100"/>
+      <c r="P4" s="103">
         <v>4.8999999999999998E-3</v>
       </c>
-      <c r="Q4" s="72">
+      <c r="Q4" s="103">
         <v>1.23E-2</v>
       </c>
-      <c r="R4" s="72">
+      <c r="R4" s="103">
         <v>0.12690000000000001</v>
       </c>
-      <c r="S4" s="72">
+      <c r="S4" s="103">
         <v>0.3291</v>
       </c>
-      <c r="T4" s="87"/>
-      <c r="U4" s="71">
+      <c r="T4" s="100"/>
+      <c r="U4" s="12">
         <v>95</v>
       </c>
     </row>
     <row r="5" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D5" s="71" t="s">
+      <c r="D5" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="71" t="s">
+      <c r="E5" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="F5" s="71">
+      <c r="F5" s="15">
         <v>50</v>
       </c>
-      <c r="G5" s="71" t="s">
+      <c r="G5" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71">
-        <v>1E-4</v>
-      </c>
-      <c r="J5" s="71">
-        <v>300</v>
-      </c>
-      <c r="K5" s="71">
+      <c r="H5" s="15"/>
+      <c r="I5" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="J5" s="15">
+        <v>200</v>
+      </c>
+      <c r="K5" s="15">
         <v>8</v>
       </c>
-      <c r="L5" s="71"/>
-      <c r="M5" s="71"/>
-      <c r="N5" s="71" t="s">
-        <v>6</v>
-      </c>
-      <c r="O5" s="87"/>
-      <c r="P5" s="72"/>
-      <c r="Q5" s="72"/>
-      <c r="R5" s="72"/>
-      <c r="S5" s="72"/>
-      <c r="T5" s="87"/>
-      <c r="U5" s="71"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5" s="100"/>
+      <c r="P5" s="64">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="Q5" s="64">
+        <v>1.1299999999999999E-2</v>
+      </c>
+      <c r="R5" s="64">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="S5" s="64">
+        <v>0.32450000000000001</v>
+      </c>
+      <c r="T5" s="100"/>
+      <c r="U5" s="15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D6" s="105" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" s="105" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" s="105">
+        <v>50</v>
+      </c>
+      <c r="G6" s="105" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="105"/>
+      <c r="I6" s="105">
+        <v>1E-4</v>
+      </c>
+      <c r="J6" s="105">
+        <v>200</v>
+      </c>
+      <c r="K6" s="105">
+        <v>8</v>
+      </c>
+      <c r="L6" s="105"/>
+      <c r="M6" s="105"/>
+      <c r="N6" s="105" t="s">
+        <v>6</v>
+      </c>
+      <c r="O6" s="100"/>
+      <c r="P6" s="110">
+        <v>1.24E-2</v>
+      </c>
+      <c r="Q6" s="110">
+        <v>1.44E-2</v>
+      </c>
+      <c r="R6" s="110">
+        <v>0.17860000000000001</v>
+      </c>
+      <c r="S6" s="110">
+        <v>0.22</v>
+      </c>
+      <c r="T6" s="100"/>
+      <c r="U6" s="111">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D7" s="104" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="104" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" s="104">
+        <v>50</v>
+      </c>
+      <c r="G7" s="104" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" s="104"/>
+      <c r="I7" s="104">
+        <v>1E-4</v>
+      </c>
+      <c r="J7" s="104">
+        <v>200</v>
+      </c>
+      <c r="K7" s="104">
+        <v>8</v>
+      </c>
+      <c r="L7" s="104"/>
+      <c r="M7" s="104"/>
+      <c r="N7" s="104" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="100"/>
+      <c r="P7" s="107">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="Q7" s="107">
+        <v>1.4E-2</v>
+      </c>
+      <c r="R7" s="107">
+        <v>0.1673</v>
+      </c>
+      <c r="S7" s="107">
+        <v>0.18149999999999999</v>
+      </c>
+      <c r="T7" s="100"/>
+      <c r="U7" s="106">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D8" s="113" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="112" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" s="113">
+        <v>50</v>
+      </c>
+      <c r="G8" s="113" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" s="114"/>
+      <c r="I8" s="113">
+        <v>1E-4</v>
+      </c>
+      <c r="J8" s="113">
+        <v>200</v>
+      </c>
+      <c r="K8" s="113">
+        <v>8</v>
+      </c>
+      <c r="L8" s="114"/>
+      <c r="M8" s="114"/>
+      <c r="N8" s="113" t="s">
+        <v>6</v>
+      </c>
+      <c r="O8" s="100"/>
+      <c r="P8" s="115"/>
+      <c r="Q8" s="115"/>
+      <c r="R8" s="115"/>
+      <c r="S8" s="115"/>
+      <c r="T8" s="100"/>
+      <c r="U8" s="116"/>
+    </row>
+    <row r="9" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D9" s="113" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="113" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="113">
+        <v>50</v>
+      </c>
+      <c r="G9" s="113" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="114"/>
+      <c r="I9" s="113">
+        <v>1E-4</v>
+      </c>
+      <c r="J9" s="113">
+        <v>200</v>
+      </c>
+      <c r="K9" s="113">
+        <v>8</v>
+      </c>
+      <c r="L9" s="114"/>
+      <c r="M9" s="114"/>
+      <c r="N9" s="113" t="s">
+        <v>6</v>
+      </c>
+      <c r="O9" s="100"/>
+      <c r="P9" s="115"/>
+      <c r="Q9" s="115"/>
+      <c r="R9" s="115"/>
+      <c r="S9" s="115"/>
+      <c r="T9" s="100"/>
+      <c r="U9" s="116"/>
+    </row>
+    <row r="10" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D10" s="117"/>
+      <c r="E10" s="118"/>
+      <c r="F10" s="118"/>
+      <c r="G10" s="118"/>
+      <c r="H10" s="118"/>
+      <c r="I10" s="118"/>
+      <c r="J10" s="118"/>
+      <c r="K10" s="118"/>
+      <c r="L10" s="118"/>
+      <c r="M10" s="118"/>
+      <c r="N10" s="118"/>
+      <c r="O10" s="100"/>
+      <c r="P10" s="119"/>
+      <c r="Q10" s="119"/>
+      <c r="R10" s="119"/>
+      <c r="S10" s="119"/>
+      <c r="T10" s="100"/>
+      <c r="U10" s="120"/>
+    </row>
+    <row r="11" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D11" s="117"/>
+      <c r="E11" s="118"/>
+      <c r="F11" s="118"/>
+      <c r="G11" s="118"/>
+      <c r="H11" s="118"/>
+      <c r="I11" s="118"/>
+      <c r="J11" s="118"/>
+      <c r="K11" s="118"/>
+      <c r="L11" s="118"/>
+      <c r="M11" s="118"/>
+      <c r="N11" s="118"/>
+      <c r="O11" s="100"/>
+      <c r="P11" s="119"/>
+      <c r="Q11" s="119"/>
+      <c r="R11" s="119"/>
+      <c r="S11" s="119"/>
+      <c r="T11" s="100"/>
+      <c r="U11" s="120"/>
+    </row>
+    <row r="12" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D12" s="121"/>
+      <c r="E12" s="122"/>
+      <c r="F12" s="122"/>
+      <c r="G12" s="122"/>
+      <c r="H12" s="122"/>
+      <c r="I12" s="122"/>
+      <c r="J12" s="122"/>
+      <c r="K12" s="122"/>
+      <c r="L12" s="122"/>
+      <c r="M12" s="122"/>
+      <c r="N12" s="122"/>
+      <c r="O12" s="100"/>
+      <c r="P12" s="123"/>
+      <c r="Q12" s="123"/>
+      <c r="R12" s="123"/>
+      <c r="S12" s="123"/>
+      <c r="T12" s="100"/>
+      <c r="U12" s="23"/>
+    </row>
+    <row r="13" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D13" s="124"/>
+      <c r="E13" s="125"/>
+      <c r="F13" s="125"/>
+      <c r="G13" s="125"/>
+      <c r="H13" s="125"/>
+      <c r="I13" s="125"/>
+      <c r="J13" s="125"/>
+      <c r="K13" s="125"/>
+      <c r="L13" s="125"/>
+      <c r="M13" s="125"/>
+      <c r="N13" s="125"/>
+      <c r="O13" s="100"/>
+      <c r="P13" s="126"/>
+      <c r="Q13" s="126"/>
+      <c r="R13" s="126"/>
+      <c r="S13" s="126"/>
+      <c r="T13" s="100"/>
+      <c r="U13" s="25"/>
+    </row>
+    <row r="14" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D14" s="71"/>
+      <c r="E14" s="101"/>
+      <c r="F14" s="101"/>
+      <c r="G14" s="101"/>
+      <c r="H14" s="101"/>
+      <c r="I14" s="101"/>
+      <c r="J14" s="101"/>
+      <c r="K14" s="101"/>
+      <c r="L14" s="101"/>
+      <c r="M14" s="101"/>
+      <c r="N14" s="101"/>
+      <c r="O14" s="100"/>
+      <c r="P14" s="72"/>
+      <c r="Q14" s="72"/>
+      <c r="R14" s="72"/>
+      <c r="S14" s="72"/>
+      <c r="T14" s="100"/>
+      <c r="U14" s="102"/>
+    </row>
+    <row r="15" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D15" s="101"/>
+      <c r="E15" s="101"/>
+      <c r="F15" s="101"/>
+      <c r="G15" s="101"/>
+      <c r="H15" s="101"/>
+      <c r="I15" s="101"/>
+      <c r="J15" s="101"/>
+      <c r="K15" s="101"/>
+      <c r="L15" s="101"/>
+      <c r="M15" s="101"/>
+      <c r="N15" s="101"/>
+      <c r="O15" s="100"/>
+      <c r="P15" s="72"/>
+      <c r="Q15" s="72"/>
+      <c r="R15" s="72"/>
+      <c r="S15" s="72"/>
+      <c r="T15" s="100"/>
+      <c r="U15" s="102"/>
+    </row>
+    <row r="16" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D16" s="101"/>
+      <c r="E16" s="101"/>
+      <c r="F16" s="101"/>
+      <c r="G16" s="101"/>
+      <c r="H16" s="101"/>
+      <c r="I16" s="101"/>
+      <c r="J16" s="101"/>
+      <c r="K16" s="101"/>
+      <c r="L16" s="101"/>
+      <c r="M16" s="101"/>
+      <c r="N16" s="101"/>
+      <c r="O16" s="100"/>
+      <c r="P16" s="72"/>
+      <c r="Q16" s="72"/>
+      <c r="R16" s="72"/>
+      <c r="S16" s="72"/>
+      <c r="T16" s="100"/>
+      <c r="U16" s="102"/>
+    </row>
+    <row r="17" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D17" s="101"/>
+      <c r="E17" s="101"/>
+      <c r="F17" s="101"/>
+      <c r="G17" s="101"/>
+      <c r="H17" s="101"/>
+      <c r="I17" s="101"/>
+      <c r="J17" s="101"/>
+      <c r="K17" s="101"/>
+      <c r="L17" s="101"/>
+      <c r="M17" s="101"/>
+      <c r="N17" s="101"/>
+      <c r="O17" s="127"/>
+      <c r="P17" s="72"/>
+      <c r="Q17" s="72"/>
+      <c r="R17" s="72"/>
+      <c r="S17" s="72"/>
+      <c r="T17" s="100"/>
+      <c r="U17" s="102"/>
+    </row>
+    <row r="18" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="P18" s="108"/>
+      <c r="Q18" s="108"/>
+      <c r="R18" s="108"/>
+      <c r="S18" s="108"/>
+      <c r="U18" s="109"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="T3:T17"/>
+    <mergeCell ref="O3:O17"/>
+  </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add - Guardado de nuevos modelos: 6_JOBO
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\MemoriaCodigoFuentev3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318123CB-65A2-467D-B874-AAAFDAD5E800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EEBD9E-73D5-4A2C-8EF2-050B35E91F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="5790" windowWidth="23310" windowHeight="7695" activeTab="3" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
+    <workbookView xWindow="2700" yWindow="4920" windowWidth="23310" windowHeight="7695" activeTab="3" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
   <sheets>
     <sheet name="full_signals - without decay" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="105">
   <si>
     <t>MODELO U-NET: FULL SIGNALS</t>
   </si>
@@ -361,10 +361,19 @@
     <t>3_DASI</t>
   </si>
   <si>
-    <t>80/21</t>
-  </si>
-  <si>
-    <t>80/22</t>
+    <t>4_DABA</t>
+  </si>
+  <si>
+    <t>5_HEFU</t>
+  </si>
+  <si>
+    <t>6_JOBO</t>
+  </si>
+  <si>
+    <t>7_ROMI</t>
+  </si>
+  <si>
+    <t>8_FEGA</t>
   </si>
 </sst>
 </file>
@@ -454,7 +463,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -593,6 +602,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFB9BB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE9FFBD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -667,7 +688,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -931,6 +952,43 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="21" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="22" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="23" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -955,76 +1013,42 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="21" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="24" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="25" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="25" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="21" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="22" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="23" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1034,6 +1058,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE9FFBD"/>
+      <color rgb="FFFFB9BB"/>
       <color rgb="FF17891A"/>
       <color rgb="FFECEECE"/>
     </mruColors>
@@ -1393,24 +1419,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="94" t="s">
+      <c r="B3" s="107" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="94"/>
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="107"/>
+      <c r="H3" s="107"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="107"/>
     </row>
     <row r="4" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -2199,10 +2225,10 @@
       <c r="P23" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q23" s="96" t="s">
+      <c r="Q23" s="109" t="s">
         <v>41</v>
       </c>
-      <c r="R23" s="97"/>
+      <c r="R23" s="110"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
@@ -2242,8 +2268,8 @@
       <c r="P24" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q24" s="98"/>
-      <c r="R24" s="97"/>
+      <c r="Q24" s="111"/>
+      <c r="R24" s="110"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
@@ -2283,8 +2309,8 @@
       <c r="P25" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q25" s="98"/>
-      <c r="R25" s="97"/>
+      <c r="Q25" s="111"/>
+      <c r="R25" s="110"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="18" t="s">
@@ -2324,8 +2350,8 @@
       <c r="P26" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q26" s="98"/>
-      <c r="R26" s="97"/>
+      <c r="Q26" s="111"/>
+      <c r="R26" s="110"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="29" t="s">
@@ -2365,8 +2391,8 @@
       <c r="P27" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q27" s="98"/>
-      <c r="R27" s="97"/>
+      <c r="Q27" s="111"/>
+      <c r="R27" s="110"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
@@ -2406,8 +2432,8 @@
       <c r="P28" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q28" s="98"/>
-      <c r="R28" s="97"/>
+      <c r="Q28" s="111"/>
+      <c r="R28" s="110"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
@@ -2447,8 +2473,8 @@
       <c r="P29" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="98"/>
-      <c r="R29" s="97"/>
+      <c r="Q29" s="111"/>
+      <c r="R29" s="110"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="18" t="s">
@@ -2488,8 +2514,8 @@
       <c r="P30" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q30" s="98"/>
-      <c r="R30" s="97"/>
+      <c r="Q30" s="111"/>
+      <c r="R30" s="110"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
@@ -2529,8 +2555,8 @@
       <c r="P31" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q31" s="98"/>
-      <c r="R31" s="97"/>
+      <c r="Q31" s="111"/>
+      <c r="R31" s="110"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="29" t="s">
@@ -2570,8 +2596,8 @@
       <c r="P32" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q32" s="98"/>
-      <c r="R32" s="97"/>
+      <c r="Q32" s="111"/>
+      <c r="R32" s="110"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
@@ -2611,8 +2637,8 @@
       <c r="P33" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q33" s="98"/>
-      <c r="R33" s="97"/>
+      <c r="Q33" s="111"/>
+      <c r="R33" s="110"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
@@ -2652,8 +2678,8 @@
       <c r="P34" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q34" s="98"/>
-      <c r="R34" s="97"/>
+      <c r="Q34" s="111"/>
+      <c r="R34" s="110"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="18" t="s">
@@ -2693,8 +2719,8 @@
       <c r="P35" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q35" s="98"/>
-      <c r="R35" s="97"/>
+      <c r="Q35" s="111"/>
+      <c r="R35" s="110"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="18" t="s">
@@ -2734,8 +2760,8 @@
       <c r="P36" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q36" s="98"/>
-      <c r="R36" s="97"/>
+      <c r="Q36" s="111"/>
+      <c r="R36" s="110"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="29" t="s">
@@ -2775,21 +2801,21 @@
       <c r="P37" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q37" s="98"/>
-      <c r="R37" s="97"/>
+      <c r="Q37" s="111"/>
+      <c r="R37" s="110"/>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B39" s="95" t="s">
+      <c r="B39" s="108" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="95"/>
-      <c r="D39" s="95"/>
-      <c r="E39" s="95"/>
-      <c r="F39" s="95"/>
-      <c r="G39" s="95"/>
-      <c r="H39" s="95"/>
-      <c r="I39" s="95"/>
-      <c r="J39" s="95"/>
+      <c r="C39" s="108"/>
+      <c r="D39" s="108"/>
+      <c r="E39" s="108"/>
+      <c r="F39" s="108"/>
+      <c r="G39" s="108"/>
+      <c r="H39" s="108"/>
+      <c r="I39" s="108"/>
+      <c r="J39" s="108"/>
     </row>
     <row r="40" spans="2:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="49" t="s">
@@ -3287,10 +3313,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="106" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="93"/>
+      <c r="C3" s="106"/>
     </row>
     <row r="5" spans="2:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="69" t="s">
@@ -3323,7 +3349,7 @@
       <c r="K5" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="99"/>
+      <c r="L5" s="112"/>
       <c r="M5" s="69" t="s">
         <v>7</v>
       </c>
@@ -3336,7 +3362,7 @@
       <c r="P5" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" s="99"/>
+      <c r="Q5" s="112"/>
       <c r="R5" s="69" t="s">
         <v>56</v>
       </c>
@@ -3369,7 +3395,7 @@
       <c r="K6" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="100"/>
+      <c r="L6" s="113"/>
       <c r="M6" s="72">
         <v>7.1400000000000005E-2</v>
       </c>
@@ -3382,7 +3408,7 @@
       <c r="P6" s="72">
         <v>0.16400000000000001</v>
       </c>
-      <c r="Q6" s="100"/>
+      <c r="Q6" s="113"/>
       <c r="R6" s="71">
         <v>116</v>
       </c>
@@ -3417,7 +3443,7 @@
       <c r="K7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="100"/>
+      <c r="L7" s="113"/>
       <c r="M7" s="75">
         <v>4.5789</v>
       </c>
@@ -3430,7 +3456,7 @@
       <c r="P7" s="75">
         <v>0.2122</v>
       </c>
-      <c r="Q7" s="100"/>
+      <c r="Q7" s="113"/>
       <c r="R7" s="6">
         <v>120</v>
       </c>
@@ -3465,7 +3491,7 @@
       <c r="K8" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="100"/>
+      <c r="L8" s="113"/>
       <c r="M8" s="72">
         <v>6.4744999999999999</v>
       </c>
@@ -3478,7 +3504,7 @@
       <c r="P8" s="72">
         <v>0.30930000000000002</v>
       </c>
-      <c r="Q8" s="100"/>
+      <c r="Q8" s="113"/>
       <c r="R8" s="71">
         <v>116</v>
       </c>
@@ -3513,7 +3539,7 @@
       <c r="K9" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L9" s="100"/>
+      <c r="L9" s="113"/>
       <c r="M9" s="72">
         <v>8.9992000000000001</v>
       </c>
@@ -3526,7 +3552,7 @@
       <c r="P9" s="72">
         <v>0.46489999999999998</v>
       </c>
-      <c r="Q9" s="100"/>
+      <c r="Q9" s="113"/>
       <c r="R9" s="71">
         <v>131</v>
       </c>
@@ -3561,7 +3587,7 @@
       <c r="K10" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="100"/>
+      <c r="L10" s="113"/>
       <c r="M10" s="72">
         <v>4.3776000000000002</v>
       </c>
@@ -3574,7 +3600,7 @@
       <c r="P10" s="72">
         <v>0.25719999999999998</v>
       </c>
-      <c r="Q10" s="100"/>
+      <c r="Q10" s="113"/>
       <c r="R10" s="71">
         <v>179</v>
       </c>
@@ -3609,7 +3635,7 @@
       <c r="K11" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="100"/>
+      <c r="L11" s="113"/>
       <c r="M11" s="72">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -3622,7 +3648,7 @@
       <c r="P11" s="72">
         <v>0.26069999999999999</v>
       </c>
-      <c r="Q11" s="100"/>
+      <c r="Q11" s="113"/>
       <c r="R11" s="71">
         <v>182</v>
       </c>
@@ -3657,7 +3683,7 @@
       <c r="K12" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="100"/>
+      <c r="L12" s="113"/>
       <c r="M12" s="72">
         <v>3.5999999999999999E-3</v>
       </c>
@@ -3670,7 +3696,7 @@
       <c r="P12" s="72">
         <v>0.39300000000000002</v>
       </c>
-      <c r="Q12" s="100"/>
+      <c r="Q12" s="113"/>
       <c r="R12" s="71">
         <v>89</v>
       </c>
@@ -3707,7 +3733,7 @@
       <c r="K13" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L13" s="100"/>
+      <c r="L13" s="113"/>
       <c r="M13" s="72">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -3720,7 +3746,7 @@
       <c r="P13" s="72">
         <v>0.41399999999999998</v>
       </c>
-      <c r="Q13" s="100"/>
+      <c r="Q13" s="113"/>
       <c r="R13" s="71">
         <v>44</v>
       </c>
@@ -3755,7 +3781,7 @@
       <c r="K14" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L14" s="100"/>
+      <c r="L14" s="113"/>
       <c r="M14" s="72">
         <v>1.1584000000000001</v>
       </c>
@@ -3768,7 +3794,7 @@
       <c r="P14" s="72">
         <v>0.1976</v>
       </c>
-      <c r="Q14" s="100"/>
+      <c r="Q14" s="113"/>
       <c r="R14" s="71">
         <v>305</v>
       </c>
@@ -3802,7 +3828,7 @@
       <c r="K15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L15" s="100"/>
+      <c r="L15" s="113"/>
       <c r="M15" s="75">
         <v>0.17349999999999999</v>
       </c>
@@ -3815,7 +3841,7 @@
       <c r="P15" s="75">
         <v>0.19939999999999999</v>
       </c>
-      <c r="Q15" s="100"/>
+      <c r="Q15" s="113"/>
       <c r="R15" s="6">
         <v>118</v>
       </c>
@@ -3849,7 +3875,7 @@
       <c r="K16" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L16" s="100"/>
+      <c r="L16" s="113"/>
       <c r="M16" s="72">
         <v>8.2579999999999991</v>
       </c>
@@ -3862,7 +3888,7 @@
       <c r="P16" s="72">
         <v>0.47870000000000001</v>
       </c>
-      <c r="Q16" s="100"/>
+      <c r="Q16" s="113"/>
       <c r="R16" s="71">
         <v>127</v>
       </c>
@@ -3892,7 +3918,7 @@
       <c r="K17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L17" s="100"/>
+      <c r="L17" s="113"/>
       <c r="M17" s="75">
         <v>3.5000000000000001E-3</v>
       </c>
@@ -3905,7 +3931,7 @@
       <c r="P17" s="75">
         <v>0.1825</v>
       </c>
-      <c r="Q17" s="100"/>
+      <c r="Q17" s="113"/>
       <c r="R17" s="6">
         <v>132</v>
       </c>
@@ -3922,12 +3948,12 @@
       <c r="I18" s="79"/>
       <c r="J18" s="79"/>
       <c r="K18" s="79"/>
-      <c r="L18" s="100"/>
+      <c r="L18" s="113"/>
       <c r="M18" s="80"/>
       <c r="N18" s="80"/>
       <c r="O18" s="80"/>
       <c r="P18" s="80"/>
-      <c r="Q18" s="100"/>
+      <c r="Q18" s="113"/>
       <c r="R18" s="81"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
@@ -3955,7 +3981,7 @@
       <c r="K19" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="L19" s="100"/>
+      <c r="L19" s="113"/>
       <c r="M19" s="85">
         <v>1.8E-3</v>
       </c>
@@ -3968,7 +3994,7 @@
       <c r="P19" s="85">
         <v>0.3236</v>
       </c>
-      <c r="Q19" s="100"/>
+      <c r="Q19" s="113"/>
       <c r="R19" s="84">
         <v>117</v>
       </c>
@@ -3998,7 +4024,7 @@
       <c r="K20" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L20" s="99"/>
+      <c r="L20" s="112"/>
       <c r="M20" s="72">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -4011,7 +4037,7 @@
       <c r="P20" s="72">
         <v>0.34599999999999997</v>
       </c>
-      <c r="Q20" s="99"/>
+      <c r="Q20" s="112"/>
       <c r="R20" s="71">
         <v>77</v>
       </c>
@@ -4027,12 +4053,12 @@
       <c r="I21" s="71"/>
       <c r="J21" s="71"/>
       <c r="K21" s="71"/>
-      <c r="L21" s="100"/>
+      <c r="L21" s="113"/>
       <c r="M21" s="72"/>
       <c r="N21" s="72"/>
       <c r="O21" s="72"/>
       <c r="P21" s="72"/>
-      <c r="Q21" s="100"/>
+      <c r="Q21" s="113"/>
       <c r="R21" s="71"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
@@ -4046,12 +4072,12 @@
       <c r="I22" s="71"/>
       <c r="J22" s="71"/>
       <c r="K22" s="71"/>
-      <c r="L22" s="100"/>
+      <c r="L22" s="113"/>
       <c r="M22" s="72"/>
       <c r="N22" s="72"/>
       <c r="O22" s="72"/>
       <c r="P22" s="72"/>
-      <c r="Q22" s="100"/>
+      <c r="Q22" s="113"/>
       <c r="R22" s="71"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
@@ -4065,12 +4091,12 @@
       <c r="I23" s="71"/>
       <c r="J23" s="71"/>
       <c r="K23" s="71"/>
-      <c r="L23" s="100"/>
+      <c r="L23" s="113"/>
       <c r="M23" s="72"/>
       <c r="N23" s="72"/>
       <c r="O23" s="72"/>
       <c r="P23" s="72"/>
-      <c r="Q23" s="100"/>
+      <c r="Q23" s="113"/>
       <c r="R23" s="71"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
@@ -4084,12 +4110,12 @@
       <c r="I24" s="71"/>
       <c r="J24" s="71"/>
       <c r="K24" s="71"/>
-      <c r="L24" s="100"/>
+      <c r="L24" s="113"/>
       <c r="M24" s="72"/>
       <c r="N24" s="72"/>
       <c r="O24" s="72"/>
       <c r="P24" s="72"/>
-      <c r="Q24" s="100"/>
+      <c r="Q24" s="113"/>
       <c r="R24" s="71"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
@@ -4103,12 +4129,12 @@
       <c r="I25" s="71"/>
       <c r="J25" s="71"/>
       <c r="K25" s="71"/>
-      <c r="L25" s="100"/>
+      <c r="L25" s="113"/>
       <c r="M25" s="72"/>
       <c r="N25" s="72"/>
       <c r="O25" s="72"/>
       <c r="P25" s="72"/>
-      <c r="Q25" s="100"/>
+      <c r="Q25" s="113"/>
       <c r="R25" s="71"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
@@ -4122,12 +4148,12 @@
       <c r="I26" s="71"/>
       <c r="J26" s="71"/>
       <c r="K26" s="71"/>
-      <c r="L26" s="100"/>
+      <c r="L26" s="113"/>
       <c r="M26" s="72"/>
       <c r="N26" s="72"/>
       <c r="O26" s="72"/>
       <c r="P26" s="72"/>
-      <c r="Q26" s="100"/>
+      <c r="Q26" s="113"/>
       <c r="R26" s="71"/>
     </row>
   </sheetData>
@@ -4693,10 +4719,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71B16EA-A98B-40B8-9C49-FBDC385B3C23}">
-  <dimension ref="D3:U18"/>
+  <dimension ref="D3:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:O17"/>
+    <sheetView tabSelected="1" topLeftCell="D9" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4712,58 +4738,63 @@
     <col min="12" max="12" width="5.5703125" customWidth="1"/>
     <col min="14" max="14" width="9.28515625" customWidth="1"/>
     <col min="15" max="15" width="4.28515625" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" customWidth="1"/>
+    <col min="18" max="18" width="8.42578125" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" customWidth="1"/>
     <col min="20" max="20" width="4.28515625" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="89" t="s">
         <v>81</v>
       </c>
-      <c r="E3" s="88" t="s">
+      <c r="E3" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="88" t="s">
+      <c r="F3" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="88" t="s">
+      <c r="G3" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="88" t="s">
+      <c r="H3" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="88" t="s">
+      <c r="I3" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="88" t="s">
+      <c r="J3" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="88" t="s">
+      <c r="K3" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="L3" s="88" t="s">
+      <c r="L3" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="M3" s="88" t="s">
+      <c r="M3" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="88" t="s">
+      <c r="N3" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="99"/>
-      <c r="P3" s="88" t="s">
+      <c r="O3" s="117"/>
+      <c r="P3" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="88" t="s">
+      <c r="Q3" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="88" t="s">
+      <c r="R3" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="88" t="s">
+      <c r="S3" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="T3" s="100"/>
-      <c r="U3" s="88" t="s">
+      <c r="T3" s="112"/>
+      <c r="U3" s="69" t="s">
         <v>56</v>
       </c>
     </row>
@@ -4795,405 +4826,878 @@
       <c r="N4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="100"/>
-      <c r="P4" s="103">
+      <c r="O4" s="118"/>
+      <c r="P4" s="93">
         <v>4.8999999999999998E-3</v>
       </c>
-      <c r="Q4" s="103">
+      <c r="Q4" s="93">
         <v>1.23E-2</v>
       </c>
-      <c r="R4" s="103">
+      <c r="R4" s="93">
         <v>0.12690000000000001</v>
       </c>
-      <c r="S4" s="103">
+      <c r="S4" s="93">
         <v>0.3291</v>
       </c>
-      <c r="T4" s="100"/>
+      <c r="T4" s="113"/>
       <c r="U4" s="12">
         <v>95</v>
       </c>
     </row>
     <row r="5" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="12">
         <v>50</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15">
-        <v>1E-4</v>
-      </c>
-      <c r="J5" s="15">
+      <c r="H5" s="12"/>
+      <c r="I5" s="12">
+        <v>1E-4</v>
+      </c>
+      <c r="J5" s="12">
         <v>200</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K5" s="12">
         <v>8</v>
       </c>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="O5" s="100"/>
-      <c r="P5" s="64">
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5" s="118"/>
+      <c r="P5" s="93">
         <v>4.5999999999999999E-3</v>
       </c>
-      <c r="Q5" s="64">
+      <c r="Q5" s="93">
         <v>1.1299999999999999E-2</v>
       </c>
-      <c r="R5" s="64">
+      <c r="R5" s="93">
         <v>0.13200000000000001</v>
       </c>
-      <c r="S5" s="64">
+      <c r="S5" s="93">
         <v>0.32450000000000001</v>
       </c>
-      <c r="T5" s="100"/>
-      <c r="U5" s="15">
+      <c r="T5" s="113"/>
+      <c r="U5" s="12">
         <v>90</v>
       </c>
     </row>
     <row r="6" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D6" s="105" t="s">
+      <c r="D6" s="94" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="105" t="s">
+      <c r="E6" s="94" t="s">
         <v>96</v>
       </c>
-      <c r="F6" s="105">
+      <c r="F6" s="94">
         <v>50</v>
       </c>
-      <c r="G6" s="105" t="s">
+      <c r="G6" s="94" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="105"/>
-      <c r="I6" s="105">
-        <v>1E-4</v>
-      </c>
-      <c r="J6" s="105">
+      <c r="H6" s="94"/>
+      <c r="I6" s="94">
+        <v>1E-4</v>
+      </c>
+      <c r="J6" s="94">
         <v>200</v>
       </c>
-      <c r="K6" s="105">
+      <c r="K6" s="94">
         <v>8</v>
       </c>
-      <c r="L6" s="105"/>
-      <c r="M6" s="105"/>
-      <c r="N6" s="105" t="s">
-        <v>6</v>
-      </c>
-      <c r="O6" s="100"/>
-      <c r="P6" s="110">
+      <c r="L6" s="94"/>
+      <c r="M6" s="94"/>
+      <c r="N6" s="94" t="s">
+        <v>6</v>
+      </c>
+      <c r="O6" s="118"/>
+      <c r="P6" s="96">
         <v>1.24E-2</v>
       </c>
-      <c r="Q6" s="110">
+      <c r="Q6" s="96">
         <v>1.44E-2</v>
       </c>
-      <c r="R6" s="110">
+      <c r="R6" s="96">
         <v>0.17860000000000001</v>
       </c>
-      <c r="S6" s="110">
+      <c r="S6" s="96">
         <v>0.22</v>
       </c>
-      <c r="T6" s="100"/>
-      <c r="U6" s="111">
+      <c r="T6" s="113"/>
+      <c r="U6" s="95">
         <v>86</v>
       </c>
     </row>
     <row r="7" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D7" s="104" t="s">
+      <c r="D7" s="94" t="s">
         <v>98</v>
       </c>
-      <c r="E7" s="104" t="s">
+      <c r="E7" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="F7" s="104">
+      <c r="F7" s="94">
         <v>50</v>
       </c>
-      <c r="G7" s="104" t="s">
+      <c r="G7" s="94" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="104"/>
-      <c r="I7" s="104">
-        <v>1E-4</v>
-      </c>
-      <c r="J7" s="104">
+      <c r="H7" s="94"/>
+      <c r="I7" s="94">
+        <v>1E-4</v>
+      </c>
+      <c r="J7" s="94">
         <v>200</v>
       </c>
-      <c r="K7" s="104">
+      <c r="K7" s="94">
         <v>8</v>
       </c>
-      <c r="L7" s="104"/>
-      <c r="M7" s="104"/>
-      <c r="N7" s="104" t="s">
-        <v>6</v>
-      </c>
-      <c r="O7" s="100"/>
-      <c r="P7" s="107">
+      <c r="L7" s="94"/>
+      <c r="M7" s="94"/>
+      <c r="N7" s="94" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="118"/>
+      <c r="P7" s="96">
         <v>1.2800000000000001E-2</v>
       </c>
-      <c r="Q7" s="107">
+      <c r="Q7" s="96">
         <v>1.4E-2</v>
       </c>
-      <c r="R7" s="107">
+      <c r="R7" s="96">
         <v>0.1673</v>
       </c>
-      <c r="S7" s="107">
+      <c r="S7" s="96">
         <v>0.18149999999999999</v>
       </c>
-      <c r="T7" s="100"/>
-      <c r="U7" s="106">
+      <c r="T7" s="113"/>
+      <c r="U7" s="95">
         <v>89</v>
       </c>
     </row>
     <row r="8" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D8" s="113" t="s">
+      <c r="D8" s="97" t="s">
         <v>99</v>
       </c>
-      <c r="E8" s="112" t="s">
+      <c r="E8" s="97" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="113">
+      <c r="F8" s="97">
         <v>50</v>
       </c>
-      <c r="G8" s="113" t="s">
+      <c r="G8" s="97" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="98"/>
+      <c r="I8" s="97">
+        <v>1E-4</v>
+      </c>
+      <c r="J8" s="97">
+        <v>200</v>
+      </c>
+      <c r="K8" s="97">
+        <v>8</v>
+      </c>
+      <c r="L8" s="98"/>
+      <c r="M8" s="98"/>
+      <c r="N8" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="O8" s="118"/>
+      <c r="P8" s="99">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="Q8" s="99">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="R8" s="99">
+        <v>0.1278</v>
+      </c>
+      <c r="S8" s="99">
+        <v>0.1338</v>
+      </c>
+      <c r="T8" s="113"/>
+      <c r="U8" s="100">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D9" s="97" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="97" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="97">
+        <v>50</v>
+      </c>
+      <c r="G9" s="97" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="98"/>
+      <c r="I9" s="97">
+        <v>1E-4</v>
+      </c>
+      <c r="J9" s="97">
+        <v>200</v>
+      </c>
+      <c r="K9" s="97">
+        <v>8</v>
+      </c>
+      <c r="L9" s="98"/>
+      <c r="M9" s="98"/>
+      <c r="N9" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="O9" s="118"/>
+      <c r="P9" s="99">
+        <v>1.12E-2</v>
+      </c>
+      <c r="Q9" s="99">
+        <v>1.03E-2</v>
+      </c>
+      <c r="R9" s="99">
+        <v>0.12280000000000001</v>
+      </c>
+      <c r="S9" s="99">
+        <v>0.12720000000000001</v>
+      </c>
+      <c r="T9" s="113"/>
+      <c r="U9" s="100">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D10" s="101" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="114"/>
-      <c r="I8" s="113">
-        <v>1E-4</v>
-      </c>
-      <c r="J8" s="113">
+      <c r="E10" s="101" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" s="101">
+        <v>50</v>
+      </c>
+      <c r="G10" s="101" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="101"/>
+      <c r="I10" s="101">
+        <v>1E-4</v>
+      </c>
+      <c r="J10" s="101">
         <v>200</v>
       </c>
-      <c r="K8" s="113">
+      <c r="K10" s="101">
         <v>8</v>
       </c>
-      <c r="L8" s="114"/>
-      <c r="M8" s="114"/>
-      <c r="N8" s="113" t="s">
-        <v>6</v>
-      </c>
-      <c r="O8" s="100"/>
-      <c r="P8" s="115"/>
-      <c r="Q8" s="115"/>
-      <c r="R8" s="115"/>
-      <c r="S8" s="115"/>
-      <c r="T8" s="100"/>
-      <c r="U8" s="116"/>
-    </row>
-    <row r="9" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D9" s="113" t="s">
-        <v>99</v>
-      </c>
-      <c r="E9" s="113" t="s">
+      <c r="L10" s="101"/>
+      <c r="M10" s="101"/>
+      <c r="N10" s="101" t="s">
+        <v>6</v>
+      </c>
+      <c r="O10" s="118"/>
+      <c r="P10" s="102">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="Q10" s="102">
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="R10" s="102">
+        <v>7.2900000000000006E-2</v>
+      </c>
+      <c r="S10" s="102">
+        <v>7.46E-2</v>
+      </c>
+      <c r="T10" s="113"/>
+      <c r="U10" s="103">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D11" s="101" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="101" t="s">
         <v>97</v>
       </c>
-      <c r="F9" s="113">
+      <c r="F11" s="101">
         <v>50</v>
       </c>
-      <c r="G9" s="113" t="s">
+      <c r="G11" s="101" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="101"/>
+      <c r="I11" s="101">
+        <v>1E-4</v>
+      </c>
+      <c r="J11" s="101">
+        <v>200</v>
+      </c>
+      <c r="K11" s="101">
+        <v>8</v>
+      </c>
+      <c r="L11" s="101"/>
+      <c r="M11" s="101"/>
+      <c r="N11" s="101" t="s">
+        <v>6</v>
+      </c>
+      <c r="O11" s="118"/>
+      <c r="P11" s="102">
+        <v>1.2200000000000001E-2</v>
+      </c>
+      <c r="Q11" s="102">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="R11" s="102">
+        <v>0.12039999999999999</v>
+      </c>
+      <c r="S11" s="102">
+        <v>6.9699999999999998E-2</v>
+      </c>
+      <c r="T11" s="113"/>
+      <c r="U11" s="103">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D12" s="104" t="s">
         <v>101</v>
       </c>
-      <c r="H9" s="114"/>
-      <c r="I9" s="113">
-        <v>1E-4</v>
-      </c>
-      <c r="J9" s="113">
+      <c r="E12" s="104" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="104">
+        <v>50</v>
+      </c>
+      <c r="G12" s="104" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="104"/>
+      <c r="I12" s="104">
+        <v>1E-4</v>
+      </c>
+      <c r="J12" s="104">
         <v>200</v>
       </c>
-      <c r="K9" s="113">
+      <c r="K12" s="104">
         <v>8</v>
       </c>
-      <c r="L9" s="114"/>
-      <c r="M9" s="114"/>
-      <c r="N9" s="113" t="s">
-        <v>6</v>
-      </c>
-      <c r="O9" s="100"/>
-      <c r="P9" s="115"/>
-      <c r="Q9" s="115"/>
-      <c r="R9" s="115"/>
-      <c r="S9" s="115"/>
-      <c r="T9" s="100"/>
-      <c r="U9" s="116"/>
-    </row>
-    <row r="10" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D10" s="117"/>
-      <c r="E10" s="118"/>
-      <c r="F10" s="118"/>
-      <c r="G10" s="118"/>
-      <c r="H10" s="118"/>
-      <c r="I10" s="118"/>
-      <c r="J10" s="118"/>
-      <c r="K10" s="118"/>
-      <c r="L10" s="118"/>
-      <c r="M10" s="118"/>
-      <c r="N10" s="118"/>
-      <c r="O10" s="100"/>
-      <c r="P10" s="119"/>
-      <c r="Q10" s="119"/>
-      <c r="R10" s="119"/>
-      <c r="S10" s="119"/>
-      <c r="T10" s="100"/>
-      <c r="U10" s="120"/>
-    </row>
-    <row r="11" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D11" s="117"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="118"/>
-      <c r="G11" s="118"/>
-      <c r="H11" s="118"/>
-      <c r="I11" s="118"/>
-      <c r="J11" s="118"/>
-      <c r="K11" s="118"/>
-      <c r="L11" s="118"/>
-      <c r="M11" s="118"/>
-      <c r="N11" s="118"/>
-      <c r="O11" s="100"/>
-      <c r="P11" s="119"/>
-      <c r="Q11" s="119"/>
-      <c r="R11" s="119"/>
-      <c r="S11" s="119"/>
-      <c r="T11" s="100"/>
-      <c r="U11" s="120"/>
-    </row>
-    <row r="12" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D12" s="121"/>
-      <c r="E12" s="122"/>
-      <c r="F12" s="122"/>
-      <c r="G12" s="122"/>
-      <c r="H12" s="122"/>
-      <c r="I12" s="122"/>
-      <c r="J12" s="122"/>
-      <c r="K12" s="122"/>
-      <c r="L12" s="122"/>
-      <c r="M12" s="122"/>
-      <c r="N12" s="122"/>
-      <c r="O12" s="100"/>
-      <c r="P12" s="123"/>
-      <c r="Q12" s="123"/>
-      <c r="R12" s="123"/>
-      <c r="S12" s="123"/>
-      <c r="T12" s="100"/>
-      <c r="U12" s="23"/>
+      <c r="L12" s="104"/>
+      <c r="M12" s="104"/>
+      <c r="N12" s="104" t="s">
+        <v>6</v>
+      </c>
+      <c r="O12" s="118"/>
+      <c r="P12" s="105">
+        <v>2.8E-3</v>
+      </c>
+      <c r="Q12" s="105">
+        <v>1.09E-2</v>
+      </c>
+      <c r="R12" s="105">
+        <v>4.9799999999999997E-2</v>
+      </c>
+      <c r="S12" s="105">
+        <v>0.2107</v>
+      </c>
+      <c r="T12" s="113"/>
+      <c r="U12" s="23">
+        <v>87</v>
+      </c>
     </row>
     <row r="13" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D13" s="124"/>
-      <c r="E13" s="125"/>
-      <c r="F13" s="125"/>
-      <c r="G13" s="125"/>
-      <c r="H13" s="125"/>
-      <c r="I13" s="125"/>
-      <c r="J13" s="125"/>
-      <c r="K13" s="125"/>
-      <c r="L13" s="125"/>
-      <c r="M13" s="125"/>
-      <c r="N13" s="125"/>
-      <c r="O13" s="100"/>
-      <c r="P13" s="126"/>
-      <c r="Q13" s="126"/>
-      <c r="R13" s="126"/>
-      <c r="S13" s="126"/>
-      <c r="T13" s="100"/>
-      <c r="U13" s="25"/>
+      <c r="D13" s="104" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="104" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13" s="104">
+        <v>50</v>
+      </c>
+      <c r="G13" s="104" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="104"/>
+      <c r="I13" s="104">
+        <v>1E-4</v>
+      </c>
+      <c r="J13" s="104">
+        <v>200</v>
+      </c>
+      <c r="K13" s="104">
+        <v>8</v>
+      </c>
+      <c r="L13" s="104"/>
+      <c r="M13" s="104"/>
+      <c r="N13" s="104" t="s">
+        <v>6</v>
+      </c>
+      <c r="O13" s="118"/>
+      <c r="P13" s="105">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="Q13" s="105">
+        <v>7.6E-3</v>
+      </c>
+      <c r="R13" s="105">
+        <v>4.58E-2</v>
+      </c>
+      <c r="S13" s="105">
+        <v>9.6600000000000005E-2</v>
+      </c>
+      <c r="T13" s="113"/>
+      <c r="U13" s="23">
+        <v>89</v>
+      </c>
     </row>
     <row r="14" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D14" s="71"/>
-      <c r="E14" s="101"/>
-      <c r="F14" s="101"/>
-      <c r="G14" s="101"/>
-      <c r="H14" s="101"/>
-      <c r="I14" s="101"/>
-      <c r="J14" s="101"/>
-      <c r="K14" s="101"/>
-      <c r="L14" s="101"/>
-      <c r="M14" s="101"/>
-      <c r="N14" s="101"/>
-      <c r="O14" s="100"/>
-      <c r="P14" s="72"/>
-      <c r="Q14" s="72"/>
-      <c r="R14" s="72"/>
-      <c r="S14" s="72"/>
-      <c r="T14" s="100"/>
-      <c r="U14" s="102"/>
+      <c r="D14" s="70" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="70" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" s="70">
+        <v>50</v>
+      </c>
+      <c r="G14" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="70"/>
+      <c r="I14" s="70">
+        <v>1E-4</v>
+      </c>
+      <c r="J14" s="70">
+        <v>200</v>
+      </c>
+      <c r="K14" s="70">
+        <v>8</v>
+      </c>
+      <c r="L14" s="70"/>
+      <c r="M14" s="70"/>
+      <c r="N14" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="O14" s="118"/>
+      <c r="P14" s="116">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="Q14" s="116">
+        <v>1.3599999999999999E-2</v>
+      </c>
+      <c r="R14" s="116">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="S14" s="116">
+        <v>0.1305</v>
+      </c>
+      <c r="T14" s="113"/>
+      <c r="U14" s="70">
+        <v>85</v>
+      </c>
     </row>
     <row r="15" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D15" s="101"/>
-      <c r="E15" s="101"/>
-      <c r="F15" s="101"/>
-      <c r="G15" s="101"/>
-      <c r="H15" s="101"/>
-      <c r="I15" s="101"/>
-      <c r="J15" s="101"/>
-      <c r="K15" s="101"/>
-      <c r="L15" s="101"/>
-      <c r="M15" s="101"/>
-      <c r="N15" s="101"/>
-      <c r="O15" s="100"/>
-      <c r="P15" s="72"/>
-      <c r="Q15" s="72"/>
-      <c r="R15" s="72"/>
-      <c r="S15" s="72"/>
-      <c r="T15" s="100"/>
-      <c r="U15" s="102"/>
+      <c r="D15" s="115" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15" s="70" t="s">
+        <v>97</v>
+      </c>
+      <c r="F15" s="70">
+        <v>50</v>
+      </c>
+      <c r="G15" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="H15" s="70"/>
+      <c r="I15" s="70">
+        <v>1E-4</v>
+      </c>
+      <c r="J15" s="70">
+        <v>200</v>
+      </c>
+      <c r="K15" s="70">
+        <v>8</v>
+      </c>
+      <c r="L15" s="70"/>
+      <c r="M15" s="70"/>
+      <c r="N15" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="O15" s="118"/>
+      <c r="P15" s="116">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="Q15" s="116">
+        <v>1.11E-2</v>
+      </c>
+      <c r="R15" s="116">
+        <v>4.3400000000000001E-2</v>
+      </c>
+      <c r="S15" s="116">
+        <v>0.11749999999999999</v>
+      </c>
+      <c r="T15" s="113"/>
+      <c r="U15" s="70">
+        <v>84</v>
+      </c>
     </row>
     <row r="16" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D16" s="101"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="101"/>
-      <c r="H16" s="101"/>
-      <c r="I16" s="101"/>
-      <c r="J16" s="101"/>
-      <c r="K16" s="101"/>
-      <c r="L16" s="101"/>
-      <c r="M16" s="101"/>
-      <c r="N16" s="101"/>
-      <c r="O16" s="100"/>
-      <c r="P16" s="72"/>
-      <c r="Q16" s="72"/>
-      <c r="R16" s="72"/>
-      <c r="S16" s="72"/>
-      <c r="T16" s="100"/>
-      <c r="U16" s="102"/>
+      <c r="D16" s="122" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" s="122" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="122">
+        <v>50</v>
+      </c>
+      <c r="G16" s="122" t="s">
+        <v>62</v>
+      </c>
+      <c r="H16" s="122"/>
+      <c r="I16" s="122">
+        <v>1E-4</v>
+      </c>
+      <c r="J16" s="122">
+        <v>200</v>
+      </c>
+      <c r="K16" s="122">
+        <v>8</v>
+      </c>
+      <c r="L16" s="122"/>
+      <c r="M16" s="122"/>
+      <c r="N16" s="122" t="s">
+        <v>6</v>
+      </c>
+      <c r="O16" s="118"/>
+      <c r="P16" s="123"/>
+      <c r="Q16" s="123"/>
+      <c r="R16" s="123"/>
+      <c r="S16" s="123"/>
+      <c r="T16" s="113"/>
+      <c r="U16" s="122"/>
     </row>
     <row r="17" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D17" s="101"/>
-      <c r="E17" s="101"/>
-      <c r="F17" s="101"/>
-      <c r="G17" s="101"/>
-      <c r="H17" s="101"/>
-      <c r="I17" s="101"/>
-      <c r="J17" s="101"/>
-      <c r="K17" s="101"/>
-      <c r="L17" s="101"/>
-      <c r="M17" s="101"/>
-      <c r="N17" s="101"/>
-      <c r="O17" s="127"/>
-      <c r="P17" s="72"/>
-      <c r="Q17" s="72"/>
-      <c r="R17" s="72"/>
-      <c r="S17" s="72"/>
-      <c r="T17" s="100"/>
-      <c r="U17" s="102"/>
+      <c r="D17" s="122" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" s="122" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" s="122">
+        <v>50</v>
+      </c>
+      <c r="G17" s="122" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="122"/>
+      <c r="I17" s="122">
+        <v>1E-4</v>
+      </c>
+      <c r="J17" s="122">
+        <v>200</v>
+      </c>
+      <c r="K17" s="122">
+        <v>8</v>
+      </c>
+      <c r="L17" s="122"/>
+      <c r="M17" s="122"/>
+      <c r="N17" s="122" t="s">
+        <v>6</v>
+      </c>
+      <c r="O17" s="118"/>
+      <c r="P17" s="123"/>
+      <c r="Q17" s="123"/>
+      <c r="R17" s="123"/>
+      <c r="S17" s="123"/>
+      <c r="T17" s="113"/>
+      <c r="U17" s="122"/>
     </row>
     <row r="18" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="P18" s="108"/>
-      <c r="Q18" s="108"/>
-      <c r="R18" s="108"/>
-      <c r="S18" s="108"/>
-      <c r="U18" s="109"/>
+      <c r="D18" s="124" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" s="124" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="124">
+        <v>50</v>
+      </c>
+      <c r="G18" s="124" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="124"/>
+      <c r="I18" s="124">
+        <v>1E-4</v>
+      </c>
+      <c r="J18" s="124">
+        <v>200</v>
+      </c>
+      <c r="K18" s="124">
+        <v>8</v>
+      </c>
+      <c r="L18" s="124"/>
+      <c r="M18" s="124"/>
+      <c r="N18" s="124" t="s">
+        <v>6</v>
+      </c>
+      <c r="O18" s="118"/>
+      <c r="P18" s="125"/>
+      <c r="Q18" s="125"/>
+      <c r="R18" s="125"/>
+      <c r="S18" s="125"/>
+      <c r="T18" s="113"/>
+      <c r="U18" s="124"/>
+    </row>
+    <row r="19" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D19" s="124" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="124" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19" s="124">
+        <v>50</v>
+      </c>
+      <c r="G19" s="124" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19" s="124"/>
+      <c r="I19" s="124">
+        <v>1E-4</v>
+      </c>
+      <c r="J19" s="124">
+        <v>200</v>
+      </c>
+      <c r="K19" s="124">
+        <v>8</v>
+      </c>
+      <c r="L19" s="124"/>
+      <c r="M19" s="124"/>
+      <c r="N19" s="124" t="s">
+        <v>6</v>
+      </c>
+      <c r="O19" s="118"/>
+      <c r="P19" s="126"/>
+      <c r="Q19" s="126"/>
+      <c r="R19" s="126"/>
+      <c r="S19" s="126"/>
+      <c r="T19" s="113"/>
+      <c r="U19" s="124"/>
+    </row>
+    <row r="20" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="71"/>
+      <c r="J20" s="71"/>
+      <c r="K20" s="71"/>
+      <c r="L20" s="71"/>
+      <c r="M20" s="71"/>
+      <c r="N20" s="71"/>
+      <c r="O20" s="118"/>
+      <c r="P20" s="121"/>
+      <c r="Q20" s="121"/>
+      <c r="R20" s="121"/>
+      <c r="S20" s="121"/>
+      <c r="T20" s="113"/>
+      <c r="U20" s="71"/>
+    </row>
+    <row r="21" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="71"/>
+      <c r="K21" s="71"/>
+      <c r="L21" s="71"/>
+      <c r="M21" s="71"/>
+      <c r="N21" s="71"/>
+      <c r="O21" s="118"/>
+      <c r="P21" s="121"/>
+      <c r="Q21" s="121"/>
+      <c r="R21" s="121"/>
+      <c r="S21" s="121"/>
+      <c r="T21" s="113"/>
+      <c r="U21" s="71"/>
+    </row>
+    <row r="22" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="71"/>
+      <c r="J22" s="71"/>
+      <c r="K22" s="71"/>
+      <c r="L22" s="71"/>
+      <c r="M22" s="71"/>
+      <c r="N22" s="71"/>
+      <c r="O22" s="118"/>
+      <c r="P22" s="121"/>
+      <c r="Q22" s="121"/>
+      <c r="R22" s="121"/>
+      <c r="S22" s="121"/>
+      <c r="T22" s="113"/>
+      <c r="U22" s="71"/>
+    </row>
+    <row r="23" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="71"/>
+      <c r="K23" s="71"/>
+      <c r="L23" s="71"/>
+      <c r="M23" s="71"/>
+      <c r="N23" s="71"/>
+      <c r="O23" s="118"/>
+      <c r="P23" s="121"/>
+      <c r="Q23" s="121"/>
+      <c r="R23" s="121"/>
+      <c r="S23" s="121"/>
+      <c r="T23" s="113"/>
+      <c r="U23" s="71"/>
+    </row>
+    <row r="24" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="71"/>
+      <c r="L24" s="71"/>
+      <c r="M24" s="71"/>
+      <c r="N24" s="71"/>
+      <c r="O24" s="118"/>
+      <c r="P24" s="121"/>
+      <c r="Q24" s="121"/>
+      <c r="R24" s="121"/>
+      <c r="S24" s="121"/>
+      <c r="T24" s="113"/>
+      <c r="U24" s="71"/>
+    </row>
+    <row r="25" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="71"/>
+      <c r="K25" s="71"/>
+      <c r="L25" s="71"/>
+      <c r="M25" s="71"/>
+      <c r="N25" s="71"/>
+      <c r="O25" s="118"/>
+      <c r="P25" s="121"/>
+      <c r="Q25" s="121"/>
+      <c r="R25" s="121"/>
+      <c r="S25" s="121"/>
+      <c r="T25" s="113"/>
+      <c r="U25" s="71"/>
+    </row>
+    <row r="26" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D26" s="71"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="71"/>
+      <c r="L26" s="71"/>
+      <c r="M26" s="71"/>
+      <c r="N26" s="71"/>
+      <c r="O26" s="118"/>
+      <c r="P26" s="121"/>
+      <c r="Q26" s="121"/>
+      <c r="R26" s="121"/>
+      <c r="S26" s="121"/>
+      <c r="T26" s="113"/>
+      <c r="U26" s="71"/>
+    </row>
+    <row r="27" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D27" s="71"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="71"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="71"/>
+      <c r="I27" s="71"/>
+      <c r="J27" s="71"/>
+      <c r="K27" s="71"/>
+      <c r="L27" s="71"/>
+      <c r="M27" s="71"/>
+      <c r="N27" s="71"/>
+      <c r="O27" s="118"/>
+      <c r="P27" s="121"/>
+      <c r="Q27" s="121"/>
+      <c r="R27" s="121"/>
+      <c r="S27" s="121"/>
+      <c r="T27" s="113"/>
+      <c r="U27" s="71"/>
+    </row>
+    <row r="28" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="71"/>
+      <c r="L28" s="71"/>
+      <c r="M28" s="71"/>
+      <c r="N28" s="71"/>
+      <c r="O28" s="118"/>
+      <c r="P28" s="121"/>
+      <c r="Q28" s="121"/>
+      <c r="R28" s="121"/>
+      <c r="S28" s="121"/>
+      <c r="T28" s="113"/>
+      <c r="U28" s="71"/>
+    </row>
+    <row r="29" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D29" s="71"/>
+      <c r="E29" s="71"/>
+      <c r="F29" s="71"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="71"/>
+      <c r="I29" s="71"/>
+      <c r="J29" s="71"/>
+      <c r="K29" s="71"/>
+      <c r="L29" s="71"/>
+      <c r="M29" s="71"/>
+      <c r="N29" s="71"/>
+      <c r="O29" s="119"/>
+      <c r="P29" s="120"/>
+      <c r="Q29" s="120"/>
+      <c r="R29" s="120"/>
+      <c r="S29" s="120"/>
+      <c r="T29" s="114"/>
+      <c r="U29" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="T3:T17"/>
-    <mergeCell ref="O3:O17"/>
+    <mergeCell ref="T3:T29"/>
+    <mergeCell ref="O3:O29"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add -Guardado de modelos
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\MemoriaCodigoFuentev3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EEBD9E-73D5-4A2C-8EF2-050B35E91F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FEE13C-08CD-4DBC-96EF-32016C50EBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="4920" windowWidth="23310" windowHeight="7695" activeTab="3" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
+    <workbookView xWindow="2700" yWindow="4920" windowWidth="23310" windowHeight="7695" firstSheet="1" activeTab="3" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
   <sheets>
     <sheet name="full_signals - without decay" sheetId="1" r:id="rId1"/>
     <sheet name="full_signals - with decay" sheetId="2" r:id="rId2"/>
     <sheet name="modelos por sujeto sano" sheetId="3" r:id="rId3"/>
-    <sheet name="Hoja1" sheetId="4" r:id="rId4"/>
+    <sheet name="SANOS-MODELS METRICS" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -989,47 +989,11 @@
     <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1049,6 +1013,42 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="25" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1419,24 +1419,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="107" t="s">
+      <c r="B3" s="116" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="116"/>
+      <c r="F3" s="116"/>
+      <c r="G3" s="116"/>
+      <c r="H3" s="116"/>
+      <c r="I3" s="116"/>
+      <c r="J3" s="116"/>
     </row>
     <row r="4" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -2225,10 +2225,10 @@
       <c r="P23" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q23" s="109" t="s">
+      <c r="Q23" s="118" t="s">
         <v>41</v>
       </c>
-      <c r="R23" s="110"/>
+      <c r="R23" s="119"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
@@ -2268,8 +2268,8 @@
       <c r="P24" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q24" s="111"/>
-      <c r="R24" s="110"/>
+      <c r="Q24" s="120"/>
+      <c r="R24" s="119"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
@@ -2309,8 +2309,8 @@
       <c r="P25" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q25" s="111"/>
-      <c r="R25" s="110"/>
+      <c r="Q25" s="120"/>
+      <c r="R25" s="119"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="18" t="s">
@@ -2350,8 +2350,8 @@
       <c r="P26" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q26" s="111"/>
-      <c r="R26" s="110"/>
+      <c r="Q26" s="120"/>
+      <c r="R26" s="119"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="29" t="s">
@@ -2391,8 +2391,8 @@
       <c r="P27" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q27" s="111"/>
-      <c r="R27" s="110"/>
+      <c r="Q27" s="120"/>
+      <c r="R27" s="119"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
@@ -2432,8 +2432,8 @@
       <c r="P28" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q28" s="111"/>
-      <c r="R28" s="110"/>
+      <c r="Q28" s="120"/>
+      <c r="R28" s="119"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
@@ -2473,8 +2473,8 @@
       <c r="P29" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="111"/>
-      <c r="R29" s="110"/>
+      <c r="Q29" s="120"/>
+      <c r="R29" s="119"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="18" t="s">
@@ -2514,8 +2514,8 @@
       <c r="P30" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q30" s="111"/>
-      <c r="R30" s="110"/>
+      <c r="Q30" s="120"/>
+      <c r="R30" s="119"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
@@ -2555,8 +2555,8 @@
       <c r="P31" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q31" s="111"/>
-      <c r="R31" s="110"/>
+      <c r="Q31" s="120"/>
+      <c r="R31" s="119"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="29" t="s">
@@ -2596,8 +2596,8 @@
       <c r="P32" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q32" s="111"/>
-      <c r="R32" s="110"/>
+      <c r="Q32" s="120"/>
+      <c r="R32" s="119"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
@@ -2637,8 +2637,8 @@
       <c r="P33" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q33" s="111"/>
-      <c r="R33" s="110"/>
+      <c r="Q33" s="120"/>
+      <c r="R33" s="119"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
@@ -2678,8 +2678,8 @@
       <c r="P34" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q34" s="111"/>
-      <c r="R34" s="110"/>
+      <c r="Q34" s="120"/>
+      <c r="R34" s="119"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="18" t="s">
@@ -2719,8 +2719,8 @@
       <c r="P35" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q35" s="111"/>
-      <c r="R35" s="110"/>
+      <c r="Q35" s="120"/>
+      <c r="R35" s="119"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="18" t="s">
@@ -2760,8 +2760,8 @@
       <c r="P36" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q36" s="111"/>
-      <c r="R36" s="110"/>
+      <c r="Q36" s="120"/>
+      <c r="R36" s="119"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="29" t="s">
@@ -2801,21 +2801,21 @@
       <c r="P37" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q37" s="111"/>
-      <c r="R37" s="110"/>
+      <c r="Q37" s="120"/>
+      <c r="R37" s="119"/>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B39" s="108" t="s">
+      <c r="B39" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="108"/>
-      <c r="D39" s="108"/>
-      <c r="E39" s="108"/>
-      <c r="F39" s="108"/>
-      <c r="G39" s="108"/>
-      <c r="H39" s="108"/>
-      <c r="I39" s="108"/>
-      <c r="J39" s="108"/>
+      <c r="C39" s="117"/>
+      <c r="D39" s="117"/>
+      <c r="E39" s="117"/>
+      <c r="F39" s="117"/>
+      <c r="G39" s="117"/>
+      <c r="H39" s="117"/>
+      <c r="I39" s="117"/>
+      <c r="J39" s="117"/>
     </row>
     <row r="40" spans="2:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="49" t="s">
@@ -3313,10 +3313,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="115" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="106"/>
+      <c r="C3" s="115"/>
     </row>
     <row r="5" spans="2:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="69" t="s">
@@ -3349,7 +3349,7 @@
       <c r="K5" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="112"/>
+      <c r="L5" s="121"/>
       <c r="M5" s="69" t="s">
         <v>7</v>
       </c>
@@ -3362,7 +3362,7 @@
       <c r="P5" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" s="112"/>
+      <c r="Q5" s="121"/>
       <c r="R5" s="69" t="s">
         <v>56</v>
       </c>
@@ -3395,7 +3395,7 @@
       <c r="K6" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="113"/>
+      <c r="L6" s="122"/>
       <c r="M6" s="72">
         <v>7.1400000000000005E-2</v>
       </c>
@@ -3408,7 +3408,7 @@
       <c r="P6" s="72">
         <v>0.16400000000000001</v>
       </c>
-      <c r="Q6" s="113"/>
+      <c r="Q6" s="122"/>
       <c r="R6" s="71">
         <v>116</v>
       </c>
@@ -3443,7 +3443,7 @@
       <c r="K7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="113"/>
+      <c r="L7" s="122"/>
       <c r="M7" s="75">
         <v>4.5789</v>
       </c>
@@ -3456,7 +3456,7 @@
       <c r="P7" s="75">
         <v>0.2122</v>
       </c>
-      <c r="Q7" s="113"/>
+      <c r="Q7" s="122"/>
       <c r="R7" s="6">
         <v>120</v>
       </c>
@@ -3491,7 +3491,7 @@
       <c r="K8" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="113"/>
+      <c r="L8" s="122"/>
       <c r="M8" s="72">
         <v>6.4744999999999999</v>
       </c>
@@ -3504,7 +3504,7 @@
       <c r="P8" s="72">
         <v>0.30930000000000002</v>
       </c>
-      <c r="Q8" s="113"/>
+      <c r="Q8" s="122"/>
       <c r="R8" s="71">
         <v>116</v>
       </c>
@@ -3539,7 +3539,7 @@
       <c r="K9" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L9" s="113"/>
+      <c r="L9" s="122"/>
       <c r="M9" s="72">
         <v>8.9992000000000001</v>
       </c>
@@ -3552,7 +3552,7 @@
       <c r="P9" s="72">
         <v>0.46489999999999998</v>
       </c>
-      <c r="Q9" s="113"/>
+      <c r="Q9" s="122"/>
       <c r="R9" s="71">
         <v>131</v>
       </c>
@@ -3587,7 +3587,7 @@
       <c r="K10" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="113"/>
+      <c r="L10" s="122"/>
       <c r="M10" s="72">
         <v>4.3776000000000002</v>
       </c>
@@ -3600,7 +3600,7 @@
       <c r="P10" s="72">
         <v>0.25719999999999998</v>
       </c>
-      <c r="Q10" s="113"/>
+      <c r="Q10" s="122"/>
       <c r="R10" s="71">
         <v>179</v>
       </c>
@@ -3635,7 +3635,7 @@
       <c r="K11" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="113"/>
+      <c r="L11" s="122"/>
       <c r="M11" s="72">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -3648,7 +3648,7 @@
       <c r="P11" s="72">
         <v>0.26069999999999999</v>
       </c>
-      <c r="Q11" s="113"/>
+      <c r="Q11" s="122"/>
       <c r="R11" s="71">
         <v>182</v>
       </c>
@@ -3683,7 +3683,7 @@
       <c r="K12" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="113"/>
+      <c r="L12" s="122"/>
       <c r="M12" s="72">
         <v>3.5999999999999999E-3</v>
       </c>
@@ -3696,7 +3696,7 @@
       <c r="P12" s="72">
         <v>0.39300000000000002</v>
       </c>
-      <c r="Q12" s="113"/>
+      <c r="Q12" s="122"/>
       <c r="R12" s="71">
         <v>89</v>
       </c>
@@ -3733,7 +3733,7 @@
       <c r="K13" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L13" s="113"/>
+      <c r="L13" s="122"/>
       <c r="M13" s="72">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -3746,7 +3746,7 @@
       <c r="P13" s="72">
         <v>0.41399999999999998</v>
       </c>
-      <c r="Q13" s="113"/>
+      <c r="Q13" s="122"/>
       <c r="R13" s="71">
         <v>44</v>
       </c>
@@ -3781,7 +3781,7 @@
       <c r="K14" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L14" s="113"/>
+      <c r="L14" s="122"/>
       <c r="M14" s="72">
         <v>1.1584000000000001</v>
       </c>
@@ -3794,7 +3794,7 @@
       <c r="P14" s="72">
         <v>0.1976</v>
       </c>
-      <c r="Q14" s="113"/>
+      <c r="Q14" s="122"/>
       <c r="R14" s="71">
         <v>305</v>
       </c>
@@ -3828,7 +3828,7 @@
       <c r="K15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L15" s="113"/>
+      <c r="L15" s="122"/>
       <c r="M15" s="75">
         <v>0.17349999999999999</v>
       </c>
@@ -3841,7 +3841,7 @@
       <c r="P15" s="75">
         <v>0.19939999999999999</v>
       </c>
-      <c r="Q15" s="113"/>
+      <c r="Q15" s="122"/>
       <c r="R15" s="6">
         <v>118</v>
       </c>
@@ -3875,7 +3875,7 @@
       <c r="K16" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L16" s="113"/>
+      <c r="L16" s="122"/>
       <c r="M16" s="72">
         <v>8.2579999999999991</v>
       </c>
@@ -3888,7 +3888,7 @@
       <c r="P16" s="72">
         <v>0.47870000000000001</v>
       </c>
-      <c r="Q16" s="113"/>
+      <c r="Q16" s="122"/>
       <c r="R16" s="71">
         <v>127</v>
       </c>
@@ -3918,7 +3918,7 @@
       <c r="K17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L17" s="113"/>
+      <c r="L17" s="122"/>
       <c r="M17" s="75">
         <v>3.5000000000000001E-3</v>
       </c>
@@ -3931,7 +3931,7 @@
       <c r="P17" s="75">
         <v>0.1825</v>
       </c>
-      <c r="Q17" s="113"/>
+      <c r="Q17" s="122"/>
       <c r="R17" s="6">
         <v>132</v>
       </c>
@@ -3948,12 +3948,12 @@
       <c r="I18" s="79"/>
       <c r="J18" s="79"/>
       <c r="K18" s="79"/>
-      <c r="L18" s="113"/>
+      <c r="L18" s="122"/>
       <c r="M18" s="80"/>
       <c r="N18" s="80"/>
       <c r="O18" s="80"/>
       <c r="P18" s="80"/>
-      <c r="Q18" s="113"/>
+      <c r="Q18" s="122"/>
       <c r="R18" s="81"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
@@ -3981,7 +3981,7 @@
       <c r="K19" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="L19" s="113"/>
+      <c r="L19" s="122"/>
       <c r="M19" s="85">
         <v>1.8E-3</v>
       </c>
@@ -3994,7 +3994,7 @@
       <c r="P19" s="85">
         <v>0.3236</v>
       </c>
-      <c r="Q19" s="113"/>
+      <c r="Q19" s="122"/>
       <c r="R19" s="84">
         <v>117</v>
       </c>
@@ -4024,7 +4024,7 @@
       <c r="K20" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L20" s="112"/>
+      <c r="L20" s="121"/>
       <c r="M20" s="72">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -4037,7 +4037,7 @@
       <c r="P20" s="72">
         <v>0.34599999999999997</v>
       </c>
-      <c r="Q20" s="112"/>
+      <c r="Q20" s="121"/>
       <c r="R20" s="71">
         <v>77</v>
       </c>
@@ -4053,12 +4053,12 @@
       <c r="I21" s="71"/>
       <c r="J21" s="71"/>
       <c r="K21" s="71"/>
-      <c r="L21" s="113"/>
+      <c r="L21" s="122"/>
       <c r="M21" s="72"/>
       <c r="N21" s="72"/>
       <c r="O21" s="72"/>
       <c r="P21" s="72"/>
-      <c r="Q21" s="113"/>
+      <c r="Q21" s="122"/>
       <c r="R21" s="71"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
@@ -4072,12 +4072,12 @@
       <c r="I22" s="71"/>
       <c r="J22" s="71"/>
       <c r="K22" s="71"/>
-      <c r="L22" s="113"/>
+      <c r="L22" s="122"/>
       <c r="M22" s="72"/>
       <c r="N22" s="72"/>
       <c r="O22" s="72"/>
       <c r="P22" s="72"/>
-      <c r="Q22" s="113"/>
+      <c r="Q22" s="122"/>
       <c r="R22" s="71"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
@@ -4091,12 +4091,12 @@
       <c r="I23" s="71"/>
       <c r="J23" s="71"/>
       <c r="K23" s="71"/>
-      <c r="L23" s="113"/>
+      <c r="L23" s="122"/>
       <c r="M23" s="72"/>
       <c r="N23" s="72"/>
       <c r="O23" s="72"/>
       <c r="P23" s="72"/>
-      <c r="Q23" s="113"/>
+      <c r="Q23" s="122"/>
       <c r="R23" s="71"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
@@ -4110,12 +4110,12 @@
       <c r="I24" s="71"/>
       <c r="J24" s="71"/>
       <c r="K24" s="71"/>
-      <c r="L24" s="113"/>
+      <c r="L24" s="122"/>
       <c r="M24" s="72"/>
       <c r="N24" s="72"/>
       <c r="O24" s="72"/>
       <c r="P24" s="72"/>
-      <c r="Q24" s="113"/>
+      <c r="Q24" s="122"/>
       <c r="R24" s="71"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
@@ -4129,12 +4129,12 @@
       <c r="I25" s="71"/>
       <c r="J25" s="71"/>
       <c r="K25" s="71"/>
-      <c r="L25" s="113"/>
+      <c r="L25" s="122"/>
       <c r="M25" s="72"/>
       <c r="N25" s="72"/>
       <c r="O25" s="72"/>
       <c r="P25" s="72"/>
-      <c r="Q25" s="113"/>
+      <c r="Q25" s="122"/>
       <c r="R25" s="71"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
@@ -4148,12 +4148,12 @@
       <c r="I26" s="71"/>
       <c r="J26" s="71"/>
       <c r="K26" s="71"/>
-      <c r="L26" s="113"/>
+      <c r="L26" s="122"/>
       <c r="M26" s="72"/>
       <c r="N26" s="72"/>
       <c r="O26" s="72"/>
       <c r="P26" s="72"/>
-      <c r="Q26" s="113"/>
+      <c r="Q26" s="122"/>
       <c r="R26" s="71"/>
     </row>
   </sheetData>
@@ -4719,6 +4719,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71B16EA-A98B-40B8-9C49-FBDC385B3C23}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="D3:U29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D9" workbookViewId="0">
@@ -4780,7 +4783,7 @@
       <c r="N3" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="117"/>
+      <c r="O3" s="124"/>
       <c r="P3" s="69" t="s">
         <v>7</v>
       </c>
@@ -4793,7 +4796,7 @@
       <c r="S3" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="T3" s="112"/>
+      <c r="T3" s="121"/>
       <c r="U3" s="69" t="s">
         <v>56</v>
       </c>
@@ -4826,7 +4829,7 @@
       <c r="N4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="118"/>
+      <c r="O4" s="125"/>
       <c r="P4" s="93">
         <v>4.8999999999999998E-3</v>
       </c>
@@ -4839,7 +4842,7 @@
       <c r="S4" s="93">
         <v>0.3291</v>
       </c>
-      <c r="T4" s="113"/>
+      <c r="T4" s="122"/>
       <c r="U4" s="12">
         <v>95</v>
       </c>
@@ -4872,7 +4875,7 @@
       <c r="N5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="118"/>
+      <c r="O5" s="125"/>
       <c r="P5" s="93">
         <v>4.5999999999999999E-3</v>
       </c>
@@ -4885,7 +4888,7 @@
       <c r="S5" s="93">
         <v>0.32450000000000001</v>
       </c>
-      <c r="T5" s="113"/>
+      <c r="T5" s="122"/>
       <c r="U5" s="12">
         <v>90</v>
       </c>
@@ -4918,7 +4921,7 @@
       <c r="N6" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="O6" s="118"/>
+      <c r="O6" s="125"/>
       <c r="P6" s="96">
         <v>1.24E-2</v>
       </c>
@@ -4931,7 +4934,7 @@
       <c r="S6" s="96">
         <v>0.22</v>
       </c>
-      <c r="T6" s="113"/>
+      <c r="T6" s="122"/>
       <c r="U6" s="95">
         <v>86</v>
       </c>
@@ -4964,7 +4967,7 @@
       <c r="N7" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="O7" s="118"/>
+      <c r="O7" s="125"/>
       <c r="P7" s="96">
         <v>1.2800000000000001E-2</v>
       </c>
@@ -4977,7 +4980,7 @@
       <c r="S7" s="96">
         <v>0.18149999999999999</v>
       </c>
-      <c r="T7" s="113"/>
+      <c r="T7" s="122"/>
       <c r="U7" s="95">
         <v>89</v>
       </c>
@@ -5010,7 +5013,7 @@
       <c r="N8" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="O8" s="118"/>
+      <c r="O8" s="125"/>
       <c r="P8" s="99">
         <v>9.4999999999999998E-3</v>
       </c>
@@ -5023,7 +5026,7 @@
       <c r="S8" s="99">
         <v>0.1338</v>
       </c>
-      <c r="T8" s="113"/>
+      <c r="T8" s="122"/>
       <c r="U8" s="100">
         <v>82</v>
       </c>
@@ -5056,7 +5059,7 @@
       <c r="N9" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="O9" s="118"/>
+      <c r="O9" s="125"/>
       <c r="P9" s="99">
         <v>1.12E-2</v>
       </c>
@@ -5069,7 +5072,7 @@
       <c r="S9" s="99">
         <v>0.12720000000000001</v>
       </c>
-      <c r="T9" s="113"/>
+      <c r="T9" s="122"/>
       <c r="U9" s="100">
         <v>82</v>
       </c>
@@ -5102,7 +5105,7 @@
       <c r="N10" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="118"/>
+      <c r="O10" s="125"/>
       <c r="P10" s="102">
         <v>1.0800000000000001E-2</v>
       </c>
@@ -5115,7 +5118,7 @@
       <c r="S10" s="102">
         <v>7.46E-2</v>
       </c>
-      <c r="T10" s="113"/>
+      <c r="T10" s="122"/>
       <c r="U10" s="103">
         <v>87</v>
       </c>
@@ -5148,7 +5151,7 @@
       <c r="N11" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="O11" s="118"/>
+      <c r="O11" s="125"/>
       <c r="P11" s="102">
         <v>1.2200000000000001E-2</v>
       </c>
@@ -5161,7 +5164,7 @@
       <c r="S11" s="102">
         <v>6.9699999999999998E-2</v>
       </c>
-      <c r="T11" s="113"/>
+      <c r="T11" s="122"/>
       <c r="U11" s="103">
         <v>86</v>
       </c>
@@ -5194,7 +5197,7 @@
       <c r="N12" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="O12" s="118"/>
+      <c r="O12" s="125"/>
       <c r="P12" s="105">
         <v>2.8E-3</v>
       </c>
@@ -5207,7 +5210,7 @@
       <c r="S12" s="105">
         <v>0.2107</v>
       </c>
-      <c r="T12" s="113"/>
+      <c r="T12" s="122"/>
       <c r="U12" s="23">
         <v>87</v>
       </c>
@@ -5240,7 +5243,7 @@
       <c r="N13" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="O13" s="118"/>
+      <c r="O13" s="125"/>
       <c r="P13" s="105">
         <v>3.5999999999999999E-3</v>
       </c>
@@ -5253,7 +5256,7 @@
       <c r="S13" s="105">
         <v>9.6600000000000005E-2</v>
       </c>
-      <c r="T13" s="113"/>
+      <c r="T13" s="122"/>
       <c r="U13" s="23">
         <v>89</v>
       </c>
@@ -5286,26 +5289,26 @@
       <c r="N14" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="O14" s="118"/>
-      <c r="P14" s="116">
+      <c r="O14" s="125"/>
+      <c r="P14" s="107">
         <v>7.3000000000000001E-3</v>
       </c>
-      <c r="Q14" s="116">
+      <c r="Q14" s="107">
         <v>1.3599999999999999E-2</v>
       </c>
-      <c r="R14" s="116">
+      <c r="R14" s="107">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="S14" s="116">
+      <c r="S14" s="107">
         <v>0.1305</v>
       </c>
-      <c r="T14" s="113"/>
+      <c r="T14" s="122"/>
       <c r="U14" s="70">
         <v>85</v>
       </c>
     </row>
     <row r="15" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D15" s="115" t="s">
+      <c r="D15" s="106" t="s">
         <v>102</v>
       </c>
       <c r="E15" s="70" t="s">
@@ -5332,167 +5335,167 @@
       <c r="N15" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="O15" s="118"/>
-      <c r="P15" s="116">
+      <c r="O15" s="125"/>
+      <c r="P15" s="107">
         <v>4.7999999999999996E-3</v>
       </c>
-      <c r="Q15" s="116">
+      <c r="Q15" s="107">
         <v>1.11E-2</v>
       </c>
-      <c r="R15" s="116">
+      <c r="R15" s="107">
         <v>4.3400000000000001E-2</v>
       </c>
-      <c r="S15" s="116">
+      <c r="S15" s="107">
         <v>0.11749999999999999</v>
       </c>
-      <c r="T15" s="113"/>
+      <c r="T15" s="122"/>
       <c r="U15" s="70">
         <v>84</v>
       </c>
     </row>
     <row r="16" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D16" s="122" t="s">
+      <c r="D16" s="110" t="s">
         <v>103</v>
       </c>
-      <c r="E16" s="122" t="s">
+      <c r="E16" s="110" t="s">
         <v>96</v>
       </c>
-      <c r="F16" s="122">
+      <c r="F16" s="110">
         <v>50</v>
       </c>
-      <c r="G16" s="122" t="s">
+      <c r="G16" s="110" t="s">
         <v>62</v>
       </c>
-      <c r="H16" s="122"/>
-      <c r="I16" s="122">
-        <v>1E-4</v>
-      </c>
-      <c r="J16" s="122">
+      <c r="H16" s="110"/>
+      <c r="I16" s="110">
+        <v>1E-4</v>
+      </c>
+      <c r="J16" s="110">
         <v>200</v>
       </c>
-      <c r="K16" s="122">
+      <c r="K16" s="110">
         <v>8</v>
       </c>
-      <c r="L16" s="122"/>
-      <c r="M16" s="122"/>
-      <c r="N16" s="122" t="s">
-        <v>6</v>
-      </c>
-      <c r="O16" s="118"/>
-      <c r="P16" s="123"/>
-      <c r="Q16" s="123"/>
-      <c r="R16" s="123"/>
-      <c r="S16" s="123"/>
-      <c r="T16" s="113"/>
-      <c r="U16" s="122"/>
+      <c r="L16" s="110"/>
+      <c r="M16" s="110"/>
+      <c r="N16" s="110" t="s">
+        <v>6</v>
+      </c>
+      <c r="O16" s="125"/>
+      <c r="P16" s="111"/>
+      <c r="Q16" s="111"/>
+      <c r="R16" s="111"/>
+      <c r="S16" s="111"/>
+      <c r="T16" s="122"/>
+      <c r="U16" s="110"/>
     </row>
     <row r="17" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D17" s="122" t="s">
+      <c r="D17" s="110" t="s">
         <v>103</v>
       </c>
-      <c r="E17" s="122" t="s">
+      <c r="E17" s="110" t="s">
         <v>97</v>
       </c>
-      <c r="F17" s="122">
+      <c r="F17" s="110">
         <v>50</v>
       </c>
-      <c r="G17" s="122" t="s">
+      <c r="G17" s="110" t="s">
         <v>62</v>
       </c>
-      <c r="H17" s="122"/>
-      <c r="I17" s="122">
-        <v>1E-4</v>
-      </c>
-      <c r="J17" s="122">
+      <c r="H17" s="110"/>
+      <c r="I17" s="110">
+        <v>1E-4</v>
+      </c>
+      <c r="J17" s="110">
         <v>200</v>
       </c>
-      <c r="K17" s="122">
+      <c r="K17" s="110">
         <v>8</v>
       </c>
-      <c r="L17" s="122"/>
-      <c r="M17" s="122"/>
-      <c r="N17" s="122" t="s">
-        <v>6</v>
-      </c>
-      <c r="O17" s="118"/>
-      <c r="P17" s="123"/>
-      <c r="Q17" s="123"/>
-      <c r="R17" s="123"/>
-      <c r="S17" s="123"/>
-      <c r="T17" s="113"/>
-      <c r="U17" s="122"/>
+      <c r="L17" s="110"/>
+      <c r="M17" s="110"/>
+      <c r="N17" s="110" t="s">
+        <v>6</v>
+      </c>
+      <c r="O17" s="125"/>
+      <c r="P17" s="111"/>
+      <c r="Q17" s="111"/>
+      <c r="R17" s="111"/>
+      <c r="S17" s="111"/>
+      <c r="T17" s="122"/>
+      <c r="U17" s="110"/>
     </row>
     <row r="18" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D18" s="124" t="s">
+      <c r="D18" s="112" t="s">
         <v>104</v>
       </c>
-      <c r="E18" s="124" t="s">
+      <c r="E18" s="112" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="124">
+      <c r="F18" s="112">
         <v>50</v>
       </c>
-      <c r="G18" s="124" t="s">
+      <c r="G18" s="112" t="s">
         <v>62</v>
       </c>
-      <c r="H18" s="124"/>
-      <c r="I18" s="124">
-        <v>1E-4</v>
-      </c>
-      <c r="J18" s="124">
+      <c r="H18" s="112"/>
+      <c r="I18" s="112">
+        <v>1E-4</v>
+      </c>
+      <c r="J18" s="112">
         <v>200</v>
       </c>
-      <c r="K18" s="124">
+      <c r="K18" s="112">
         <v>8</v>
       </c>
-      <c r="L18" s="124"/>
-      <c r="M18" s="124"/>
-      <c r="N18" s="124" t="s">
-        <v>6</v>
-      </c>
-      <c r="O18" s="118"/>
-      <c r="P18" s="125"/>
-      <c r="Q18" s="125"/>
-      <c r="R18" s="125"/>
-      <c r="S18" s="125"/>
-      <c r="T18" s="113"/>
-      <c r="U18" s="124"/>
+      <c r="L18" s="112"/>
+      <c r="M18" s="112"/>
+      <c r="N18" s="112" t="s">
+        <v>6</v>
+      </c>
+      <c r="O18" s="125"/>
+      <c r="P18" s="113"/>
+      <c r="Q18" s="113"/>
+      <c r="R18" s="113"/>
+      <c r="S18" s="113"/>
+      <c r="T18" s="122"/>
+      <c r="U18" s="112"/>
     </row>
     <row r="19" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D19" s="124" t="s">
+      <c r="D19" s="112" t="s">
         <v>104</v>
       </c>
-      <c r="E19" s="124" t="s">
+      <c r="E19" s="112" t="s">
         <v>97</v>
       </c>
-      <c r="F19" s="124">
+      <c r="F19" s="112">
         <v>50</v>
       </c>
-      <c r="G19" s="124" t="s">
+      <c r="G19" s="112" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="124"/>
-      <c r="I19" s="124">
-        <v>1E-4</v>
-      </c>
-      <c r="J19" s="124">
+      <c r="H19" s="112"/>
+      <c r="I19" s="112">
+        <v>1E-4</v>
+      </c>
+      <c r="J19" s="112">
         <v>200</v>
       </c>
-      <c r="K19" s="124">
+      <c r="K19" s="112">
         <v>8</v>
       </c>
-      <c r="L19" s="124"/>
-      <c r="M19" s="124"/>
-      <c r="N19" s="124" t="s">
-        <v>6</v>
-      </c>
-      <c r="O19" s="118"/>
-      <c r="P19" s="126"/>
-      <c r="Q19" s="126"/>
-      <c r="R19" s="126"/>
-      <c r="S19" s="126"/>
-      <c r="T19" s="113"/>
-      <c r="U19" s="124"/>
+      <c r="L19" s="112"/>
+      <c r="M19" s="112"/>
+      <c r="N19" s="112" t="s">
+        <v>6</v>
+      </c>
+      <c r="O19" s="125"/>
+      <c r="P19" s="114"/>
+      <c r="Q19" s="114"/>
+      <c r="R19" s="114"/>
+      <c r="S19" s="114"/>
+      <c r="T19" s="122"/>
+      <c r="U19" s="112"/>
     </row>
     <row r="20" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D20" s="71"/>
@@ -5506,12 +5509,12 @@
       <c r="L20" s="71"/>
       <c r="M20" s="71"/>
       <c r="N20" s="71"/>
-      <c r="O20" s="118"/>
-      <c r="P20" s="121"/>
-      <c r="Q20" s="121"/>
-      <c r="R20" s="121"/>
-      <c r="S20" s="121"/>
-      <c r="T20" s="113"/>
+      <c r="O20" s="125"/>
+      <c r="P20" s="109"/>
+      <c r="Q20" s="109"/>
+      <c r="R20" s="109"/>
+      <c r="S20" s="109"/>
+      <c r="T20" s="122"/>
       <c r="U20" s="71"/>
     </row>
     <row r="21" spans="4:21" x14ac:dyDescent="0.25">
@@ -5526,12 +5529,12 @@
       <c r="L21" s="71"/>
       <c r="M21" s="71"/>
       <c r="N21" s="71"/>
-      <c r="O21" s="118"/>
-      <c r="P21" s="121"/>
-      <c r="Q21" s="121"/>
-      <c r="R21" s="121"/>
-      <c r="S21" s="121"/>
-      <c r="T21" s="113"/>
+      <c r="O21" s="125"/>
+      <c r="P21" s="109"/>
+      <c r="Q21" s="109"/>
+      <c r="R21" s="109"/>
+      <c r="S21" s="109"/>
+      <c r="T21" s="122"/>
       <c r="U21" s="71"/>
     </row>
     <row r="22" spans="4:21" x14ac:dyDescent="0.25">
@@ -5546,12 +5549,12 @@
       <c r="L22" s="71"/>
       <c r="M22" s="71"/>
       <c r="N22" s="71"/>
-      <c r="O22" s="118"/>
-      <c r="P22" s="121"/>
-      <c r="Q22" s="121"/>
-      <c r="R22" s="121"/>
-      <c r="S22" s="121"/>
-      <c r="T22" s="113"/>
+      <c r="O22" s="125"/>
+      <c r="P22" s="109"/>
+      <c r="Q22" s="109"/>
+      <c r="R22" s="109"/>
+      <c r="S22" s="109"/>
+      <c r="T22" s="122"/>
       <c r="U22" s="71"/>
     </row>
     <row r="23" spans="4:21" x14ac:dyDescent="0.25">
@@ -5566,12 +5569,12 @@
       <c r="L23" s="71"/>
       <c r="M23" s="71"/>
       <c r="N23" s="71"/>
-      <c r="O23" s="118"/>
-      <c r="P23" s="121"/>
-      <c r="Q23" s="121"/>
-      <c r="R23" s="121"/>
-      <c r="S23" s="121"/>
-      <c r="T23" s="113"/>
+      <c r="O23" s="125"/>
+      <c r="P23" s="109"/>
+      <c r="Q23" s="109"/>
+      <c r="R23" s="109"/>
+      <c r="S23" s="109"/>
+      <c r="T23" s="122"/>
       <c r="U23" s="71"/>
     </row>
     <row r="24" spans="4:21" x14ac:dyDescent="0.25">
@@ -5586,12 +5589,12 @@
       <c r="L24" s="71"/>
       <c r="M24" s="71"/>
       <c r="N24" s="71"/>
-      <c r="O24" s="118"/>
-      <c r="P24" s="121"/>
-      <c r="Q24" s="121"/>
-      <c r="R24" s="121"/>
-      <c r="S24" s="121"/>
-      <c r="T24" s="113"/>
+      <c r="O24" s="125"/>
+      <c r="P24" s="109"/>
+      <c r="Q24" s="109"/>
+      <c r="R24" s="109"/>
+      <c r="S24" s="109"/>
+      <c r="T24" s="122"/>
       <c r="U24" s="71"/>
     </row>
     <row r="25" spans="4:21" x14ac:dyDescent="0.25">
@@ -5606,12 +5609,12 @@
       <c r="L25" s="71"/>
       <c r="M25" s="71"/>
       <c r="N25" s="71"/>
-      <c r="O25" s="118"/>
-      <c r="P25" s="121"/>
-      <c r="Q25" s="121"/>
-      <c r="R25" s="121"/>
-      <c r="S25" s="121"/>
-      <c r="T25" s="113"/>
+      <c r="O25" s="125"/>
+      <c r="P25" s="109"/>
+      <c r="Q25" s="109"/>
+      <c r="R25" s="109"/>
+      <c r="S25" s="109"/>
+      <c r="T25" s="122"/>
       <c r="U25" s="71"/>
     </row>
     <row r="26" spans="4:21" x14ac:dyDescent="0.25">
@@ -5626,12 +5629,12 @@
       <c r="L26" s="71"/>
       <c r="M26" s="71"/>
       <c r="N26" s="71"/>
-      <c r="O26" s="118"/>
-      <c r="P26" s="121"/>
-      <c r="Q26" s="121"/>
-      <c r="R26" s="121"/>
-      <c r="S26" s="121"/>
-      <c r="T26" s="113"/>
+      <c r="O26" s="125"/>
+      <c r="P26" s="109"/>
+      <c r="Q26" s="109"/>
+      <c r="R26" s="109"/>
+      <c r="S26" s="109"/>
+      <c r="T26" s="122"/>
       <c r="U26" s="71"/>
     </row>
     <row r="27" spans="4:21" x14ac:dyDescent="0.25">
@@ -5646,12 +5649,12 @@
       <c r="L27" s="71"/>
       <c r="M27" s="71"/>
       <c r="N27" s="71"/>
-      <c r="O27" s="118"/>
-      <c r="P27" s="121"/>
-      <c r="Q27" s="121"/>
-      <c r="R27" s="121"/>
-      <c r="S27" s="121"/>
-      <c r="T27" s="113"/>
+      <c r="O27" s="125"/>
+      <c r="P27" s="109"/>
+      <c r="Q27" s="109"/>
+      <c r="R27" s="109"/>
+      <c r="S27" s="109"/>
+      <c r="T27" s="122"/>
       <c r="U27" s="71"/>
     </row>
     <row r="28" spans="4:21" x14ac:dyDescent="0.25">
@@ -5666,12 +5669,12 @@
       <c r="L28" s="71"/>
       <c r="M28" s="71"/>
       <c r="N28" s="71"/>
-      <c r="O28" s="118"/>
-      <c r="P28" s="121"/>
-      <c r="Q28" s="121"/>
-      <c r="R28" s="121"/>
-      <c r="S28" s="121"/>
-      <c r="T28" s="113"/>
+      <c r="O28" s="125"/>
+      <c r="P28" s="109"/>
+      <c r="Q28" s="109"/>
+      <c r="R28" s="109"/>
+      <c r="S28" s="109"/>
+      <c r="T28" s="122"/>
       <c r="U28" s="71"/>
     </row>
     <row r="29" spans="4:21" x14ac:dyDescent="0.25">
@@ -5686,12 +5689,12 @@
       <c r="L29" s="71"/>
       <c r="M29" s="71"/>
       <c r="N29" s="71"/>
-      <c r="O29" s="119"/>
-      <c r="P29" s="120"/>
-      <c r="Q29" s="120"/>
-      <c r="R29" s="120"/>
-      <c r="S29" s="120"/>
-      <c r="T29" s="114"/>
+      <c r="O29" s="126"/>
+      <c r="P29" s="108"/>
+      <c r="Q29" s="108"/>
+      <c r="R29" s="108"/>
+      <c r="S29" s="108"/>
+      <c r="T29" s="123"/>
       <c r="U29" s="71"/>
     </row>
   </sheetData>

</xml_diff>